<commit_message>
Skill information translation. (~30)
</commit_message>
<xml_diff>
--- a/skill.xlsx
+++ b/skill.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19120"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="179016"/>
 </workbook>
 </file>
 
@@ -28,280 +28,286 @@
     <t>effect</t>
   </si>
   <si>
-    <t>荒鉤爪</t>
-  </si>
-  <si>
-    <t>荒鉤爪の魂</t>
+    <t>황구조(荒鉤爪)</t>
+  </si>
+  <si>
+    <t>황구조의 혼(荒鉤爪の魂)</t>
   </si>
   <si>
     <t>10</t>
   </si>
   <si>
-    <t>早食い+2 + 高級耳栓</t>
-  </si>
-  <si>
-    <t>居合</t>
-  </si>
-  <si>
-    <t>居合術【力】</t>
-  </si>
-  <si>
-    <t>抜刀術【力】 + 納刀術</t>
-  </si>
-  <si>
-    <t>怒</t>
-  </si>
-  <si>
-    <t>逆鱗</t>
-  </si>
-  <si>
-    <t>火事場力+2 + 根性</t>
-  </si>
-  <si>
-    <t>岩穿</t>
-  </si>
-  <si>
-    <t>岩穿の魂</t>
-  </si>
-  <si>
-    <t>火事場力+2 + 拾い食い</t>
-  </si>
-  <si>
-    <t>泡沫</t>
-  </si>
-  <si>
-    <t>泡沫の舞</t>
-  </si>
-  <si>
-    <t>泡状態【大】にならない。回避行動を繰り返すと泡状態【小】になり、回避時の無敵時間が伸び、スタミナ消費減少することがある</t>
-  </si>
-  <si>
-    <t>裏会心</t>
-  </si>
-  <si>
-    <t>痛恨会心</t>
-  </si>
-  <si>
-    <t>マイナス会心攻撃時に25%の確率で与えるダメージが2倍になる。</t>
-  </si>
-  <si>
-    <t>裏稼業</t>
-  </si>
-  <si>
-    <t>暗躍</t>
-  </si>
-  <si>
-    <t>装填数UP + 調合成功率+20% + 隠密</t>
-  </si>
-  <si>
-    <t>運気</t>
-  </si>
-  <si>
-    <t>激運/強運/幸運/不運/災難</t>
+    <t>속식+2(早食い+2) + 고급 귀마개(高級耳栓)</t>
+  </si>
+  <si>
+    <t>거합(居合)</t>
+  </si>
+  <si>
+    <t>거합술【력】(居合術【力】)</t>
+  </si>
+  <si>
+    <t>발도술【력】(抜刀術【力】) + 납도술(納刀術)</t>
+  </si>
+  <si>
+    <t>노(怒)</t>
+  </si>
+  <si>
+    <t>역린(逆鱗)</t>
+  </si>
+  <si>
+    <t>화사장력+2(火事場力+2) + 근성(根性)</t>
+  </si>
+  <si>
+    <t>암천(岩穿)</t>
+  </si>
+  <si>
+    <t>암천의 혼(岩穿の魂)</t>
+  </si>
+  <si>
+    <t>화사장력+2(火事場力+2) + 주워먹기(拾い食い)</t>
+  </si>
+  <si>
+    <t>포말(泡沫)</t>
+  </si>
+  <si>
+    <t>포말의 춤(泡沫の舞)</t>
+  </si>
+  <si>
+    <t>거품상태【대】가 되지 않는다.
+회피행동을 반복(통상회피 3회, 스텝회피4회)하면 거품상태【소】가 되어 회피시의 무적시간이 늘어나고 스태미너 소비가 감소한다.
+(회피성능+1, 체술+1)</t>
+  </si>
+  <si>
+    <t>역회심(裏会心)</t>
+  </si>
+  <si>
+    <t>통한회심(痛恨会心)</t>
+  </si>
+  <si>
+    <t>마이너스 회심공격시에 25%의 확률로 데미지가 2배가 된다.</t>
+  </si>
+  <si>
+    <t>비밀공작(裏稼業)</t>
+  </si>
+  <si>
+    <t>암약(暗躍)</t>
+  </si>
+  <si>
+    <t>장전수UP(装填数UP) + 조합성공률+20%(調合成功率+20%) + 은밀(隠密)</t>
+  </si>
+  <si>
+    <t>운신(運気)</t>
+  </si>
+  <si>
+    <t>격운(激運)/강운(強運)/행운(幸運)/불운(不運)/재난(災難)</t>
   </si>
   <si>
     <t>20/15/10/-10/-15</t>
   </si>
   <si>
-    <t>クエストクリア報酬の抽選で報酬を入手できる確率が通常の22/32から31/32になる。/クエストクリア報酬の抽選で報酬を入手できる確率が通常の22/32から28/32になる。/クエストクリア報酬の抽選で報酬を入手できる確率が通常の22/32から25/32になる。/クエストクリア報酬の抽選で報酬を入手できる確率が通常の22/32から16/32になる。/クエストクリア報酬の抽選で報酬を入手できる確率が通常の22/32から8/32になる。</t>
-  </si>
-  <si>
-    <t>運搬</t>
-  </si>
-  <si>
-    <t>運搬の達人</t>
-  </si>
-  <si>
-    <t>運搬時の移動速度が上昇。高いところから飛び降りても運搬物を落としにくくなる</t>
-  </si>
-  <si>
-    <t>英雄の盾</t>
-  </si>
-  <si>
-    <t>英雄の護り</t>
-  </si>
-  <si>
-    <t>小ダメージ(5以下)を無効化。状態異常、アイテム、徐々に体力が減る攻撃は無効化出来ない</t>
-  </si>
-  <si>
-    <t>ＳＰ延長</t>
-  </si>
-  <si>
-    <t>ＳＰ時間延長</t>
-  </si>
-  <si>
-    <t>ＳＰ狩技で発動するＳＰ状態の効果時間が1.25倍になる</t>
-  </si>
-  <si>
-    <t>炎熱適応</t>
-  </si>
-  <si>
-    <t>南風の狩人</t>
-  </si>
-  <si>
-    <t>暑さ無効と暑い場所で攻撃力15と防御力20上昇。ホットドリンクでさらに防御力10アップ</t>
-  </si>
-  <si>
-    <t>鏖魔</t>
-  </si>
-  <si>
-    <t>鏖魔の魂</t>
-  </si>
-  <si>
-    <t>攻撃力UP【大】 + 回避性能+2</t>
-  </si>
-  <si>
-    <t>大雪主</t>
-  </si>
-  <si>
-    <t>大雪主の魂</t>
-  </si>
-  <si>
-    <t>回避距離UP + スタミナ急速回復</t>
-  </si>
-  <si>
-    <t>朧隠</t>
-  </si>
-  <si>
-    <t>朧隠の魂</t>
-  </si>
-  <si>
-    <t>高級耳栓 + 装填速度+3 + 心剣一体</t>
-  </si>
-  <si>
-    <t>ガード強化</t>
-  </si>
-  <si>
-    <t>通常ガード不能の攻撃がガードできるようになる。特定の攻撃をガードした時に一部アイテム使用不可状態、防御DOWN状態にならない</t>
-  </si>
-  <si>
-    <t>ガード性能</t>
-  </si>
-  <si>
-    <t>ガード性能+2/ガード性能+1/ガード性能-1</t>
+    <t>퀘스트 클리어 보수의 추첨에서 보수를 입수할 수 있는 확률이 통상의 22/32에서 31/32이 된다.
+/퀘스트 클리어 보수의 추첨에서 보수를 입수할 수 있는 확률이 통상의 22/32에서 28/32이 된다.
+/퀘스트 클리어 보수의 추첨에서 보수를 입수할 수 있는 확률이 통상의 22/32에서 25/32이 된다.
+/퀘스트 클리어 보수의 추첨에서 보수를 입수할 수 있는 확률이 통상의 22/32에서 16/32이 된다.
+/퀘스트 클리어 보수의 추첨에서 보수를 입수할 수 있는 확률이 통상의 22/32에서 8/32이 된다.</t>
+  </si>
+  <si>
+    <t>운반(運搬)</t>
+  </si>
+  <si>
+    <t>운반의 달인(運搬の達人)</t>
+  </si>
+  <si>
+    <t>운반시의 이동속도가 상승. 높은 곳에서 뛰어 내려도 운반물을 잘 떨어뜨리지 않게 된다.</t>
+  </si>
+  <si>
+    <t>영웅의 방패(英雄の盾)</t>
+  </si>
+  <si>
+    <t>영웅의 수호(英雄の護り)</t>
+  </si>
+  <si>
+    <t>작은 데미지(5이하)를 무효화. 상태이상, 아이템, 도트데미지 공격은 무효화 불가능</t>
+  </si>
+  <si>
+    <t>SP연장(ＳＰ延長)</t>
+  </si>
+  <si>
+    <t>SP시간연장(ＳＰ時間延長)</t>
+  </si>
+  <si>
+    <t>SP수기로 발동하는 SP상태의 효과시간이 1.25배가 된다.</t>
+  </si>
+  <si>
+    <t>염열적응(炎熱適応)</t>
+  </si>
+  <si>
+    <t>남풍의 사냥꾼(南風の狩人)</t>
+  </si>
+  <si>
+    <t>더위 무효와 뜨거운 장소에서 공격력15와 방어력20상승. 핫드링크를 마시면 추가로 방어력10 상승</t>
+  </si>
+  <si>
+    <t>오마(鏖魔)</t>
+  </si>
+  <si>
+    <t>오마의 혼(鏖魔の魂)</t>
+  </si>
+  <si>
+    <t>공격력UP【大】(攻撃力UP【大】) + 회피성능+2(回避性能+2)</t>
+  </si>
+  <si>
+    <t>대설주(大雪主)</t>
+  </si>
+  <si>
+    <t>대설주의 혼(大雪主の魂)</t>
+  </si>
+  <si>
+    <t>회피거리UP(回避距離UP) + 스태미너 급속회복(スタミナ急速回復)</t>
+  </si>
+  <si>
+    <t>농은(朧隠)</t>
+  </si>
+  <si>
+    <t>농은의 혼(朧隠の魂)</t>
+  </si>
+  <si>
+    <t>고급 귀마개(高級耳栓) + 장전속도+3(装填速度+3) + 심검일체(心剣一体)</t>
+  </si>
+  <si>
+    <t>가드강화(ガード強化)</t>
+  </si>
+  <si>
+    <t>통상 가드 불가능한 공격이 가드 가능하게 된다. 특정 공격을 가드했을 때 일부 아이템 사용불가상태, 방어DOWN 상태가 되지 않는다.</t>
+  </si>
+  <si>
+    <t>가드성능(ガード性能)</t>
+  </si>
+  <si>
+    <t>가드성능+2(ガード性能+2)/가드성능+1(ガード性能+1)/가드성능-1(ガード性能-1)</t>
   </si>
   <si>
     <t>15/10/-10</t>
   </si>
   <si>
-    <t>ガードした時の後退を抑え、ガード時の威力を20軽減/ガードした時の後退を抑え、ガード時の威力を10軽減/ガードした時に後退しやすくなり、ガード時の威力が10増える</t>
-  </si>
-  <si>
-    <t>会心強化</t>
-  </si>
-  <si>
-    <t>超会心</t>
-  </si>
-  <si>
-    <t>会心時のダメージが通常の1.25倍から1.4倍に増加する</t>
-  </si>
-  <si>
-    <t>回避距離</t>
-  </si>
-  <si>
-    <t>回避距離UP</t>
-  </si>
-  <si>
-    <t>回転回避やステップの移動距離が1.5倍に伸びる</t>
-  </si>
-  <si>
-    <t>回避術</t>
-  </si>
-  <si>
-    <t>軽業師</t>
-  </si>
-  <si>
-    <t>体術+1 + 回避性能+1</t>
-  </si>
-  <si>
-    <t>回避性能</t>
-  </si>
-  <si>
-    <t>回避性能+2/回避性能+1/回避性能DOWN</t>
-  </si>
-  <si>
-    <t>回転回避やステップの無敵時間が通常の0.2秒から0.4秒に延長される/回転回避やステップの無敵時間が通常の0.2秒から0.33秒に延長される/回転回避やステップの無敵時間が通常の0.2秒から0.1秒に短縮される</t>
-  </si>
-  <si>
-    <t>回復速度</t>
-  </si>
-  <si>
-    <t>回復速度+2/回復速度+1/回復速度-1/回復速度-2</t>
+    <t>가드 시 밀림 방지, 가드 시 위력 20경감/가드 시 밀림 방지, 가드 시 위력 10경감/가드 시 밀리기 쉬워짐, 가드 시 위력 20증가</t>
+  </si>
+  <si>
+    <t>회심강화(会心強化)</t>
+  </si>
+  <si>
+    <t>초회심(超会心)</t>
+  </si>
+  <si>
+    <t>회심 시 데미지가 통상의 1.25배에서 1.4배로 증가한다.</t>
+  </si>
+  <si>
+    <t>회피거리(回避距離)</t>
+  </si>
+  <si>
+    <t>회피거리UP(回避距離UP)</t>
+  </si>
+  <si>
+    <t>구르기나 스텝의 이동거리가 1.5배로 늘어난다.</t>
+  </si>
+  <si>
+    <t>회피술(回避術)</t>
+  </si>
+  <si>
+    <t>곡예사(軽業師)</t>
+  </si>
+  <si>
+    <t>체술+1(体術+1) + 회피성능+1(回避性能+1)</t>
+  </si>
+  <si>
+    <t>회피성능(回避性能)</t>
+  </si>
+  <si>
+    <t>회피성능+2(回避性能+2)/회피성능+1(回避性能+1)/회피성능DOWN(回避性能DOWN)</t>
+  </si>
+  <si>
+    <t>구르기나 스텝의 무적시간이 통상의 0.2초에서 0.4초로 연장된다./구르기나 스텝의 무적시간이 통상의 0.2초에서 0.33초로 연장된다./구르기나 스텝의 무적시간이 통상의 0.2초에서 0.1초로 단축된다.</t>
+  </si>
+  <si>
+    <t>회복속도(回復速度)</t>
+  </si>
+  <si>
+    <t>회복속도+2(回復速度+2)/회복속도+1(回復速度+1)/회복속도-1(回復速度-1)/회복속도-2(回復速度-2)</t>
   </si>
   <si>
     <t>15/10/-10/-15</t>
   </si>
   <si>
-    <t>赤ゲージの回復速度が4倍になる/赤ゲージの回復速度が2倍になる/赤ゲージの回復速度が1/2になる/赤ゲージの回復速度が1/4になる</t>
-  </si>
-  <si>
-    <t>回復量</t>
-  </si>
-  <si>
-    <t>体力回復量UP/体力回復量DOWN</t>
+    <t>붉은 게이지의 회복속도가 4배가 된다/붉은 게이지의 회복속도가 2배가 된다/붉은 게이지의 회복속도가 1/2이 된다/붉은 게이지의 회복속도가 1/4이 된다</t>
+  </si>
+  <si>
+    <t>회복량(回復量)</t>
+  </si>
+  <si>
+    <t>체력회복량UP(体力回復量UP)/체력회복량DOWN(体力回復量DOWN)</t>
   </si>
   <si>
     <t>10/-10</t>
   </si>
   <si>
-    <t>体力回復アイテムの回復量が1.25倍に増える/体力回復アイテムの回復量が0.75倍に減る</t>
-  </si>
-  <si>
-    <t>拡散弾追加</t>
-  </si>
-  <si>
-    <t>拡散弾全LV追加/拡散弾LV1追加</t>
+    <t>체력회복 아이템의 회복량이 1.25배로 늘어난다./체력회복 아이템의 회복량이 0.75배로 줄어든다.</t>
+  </si>
+  <si>
+    <t>확산탄추가(拡散弾追加)</t>
+  </si>
+  <si>
+    <t>확산탄 전LV 추가(拡散弾全LV追加)/확산탄 LV1 추가(拡散弾LV1追加)</t>
   </si>
   <si>
     <t>15/10</t>
   </si>
   <si>
-    <t>全LVの拡散弾が使えるようになる/LV1拡散弾が使えるようになる</t>
-  </si>
-  <si>
-    <t>加護</t>
-  </si>
-  <si>
-    <t>精霊の加護/悪霊の加護</t>
-  </si>
-  <si>
-    <t>1/4の確率で受けるダメージが30%減少する/1/4の確率で受けるダメージが30%増加する</t>
-  </si>
-  <si>
-    <t>我慢</t>
-  </si>
-  <si>
-    <t>虎視眈々</t>
-  </si>
-  <si>
-    <t>モンスターからのダメージでも狩技、ブレイヴ(ダメージの2倍)、レンキンゲージが溜まる。ストライカーの場合は狩技ゲージの蓄積量がダメージの1.4倍</t>
-  </si>
-  <si>
-    <t>雷属性攻撃</t>
-  </si>
-  <si>
-    <t>雷属性攻撃強化+2/雷属性攻撃強化+1/雷属性攻撃弱化</t>
-  </si>
-  <si>
-    <t>雷属性の攻撃が1.1倍+6になる/雷属性の攻撃が1.05倍+4になる/雷属性の攻撃が0.75倍になる</t>
-  </si>
-  <si>
-    <t>雷耐性</t>
-  </si>
-  <si>
-    <t>雷耐性【大】/雷耐性【小】/雷耐性弱化</t>
+    <t>전LV의 확산탄을 사용할 수 있게 된다./LV1확산탄을 사용할 수 있게 된다.</t>
+  </si>
+  <si>
+    <t>가호(加護)</t>
+  </si>
+  <si>
+    <t>정령의 가호(精霊の加護)/악령의 가호(悪霊の加護)</t>
+  </si>
+  <si>
+    <t>1/4의 확률로 받는 데미지가 30% 감소한다./1/4의 확률로 받는 데미지가 30% 증가한다.</t>
+  </si>
+  <si>
+    <t>참기(我慢)</t>
+  </si>
+  <si>
+    <t>호시탐탐(虎視眈々)</t>
+  </si>
+  <si>
+    <t>몬스터로부터 데미지를 받을 때 수기, 브레이브(데미지의 2배), 연금게이지가 쌓인다. 스트라이커의 경우 수기 게이지의 축적량이 데미지의 1.4배</t>
+  </si>
+  <si>
+    <t>뇌속성 공격(雷属性攻撃)</t>
+  </si>
+  <si>
+    <t>뇌속성 공격 강화+2(雷属性攻撃強化+2)/뇌속성 공격 강화+1(雷属性攻撃強化+1)/뇌속성 공격 약화(雷属性攻撃弱化)</t>
+  </si>
+  <si>
+    <t>뇌속성의 공격이 1.1배+5이 된다./뇌속성의 공격이 1.05배+4가 된다./뇌속성의 공격이 0.75배가 된다.</t>
+  </si>
+  <si>
+    <t>뇌내성(雷耐性)</t>
+  </si>
+  <si>
+    <t>뇌내성【대】(雷耐性【大】)/뇌내성【소】(雷耐性【小】)/뇌내성 약화(雷耐性弱化)</t>
   </si>
   <si>
     <t>雷耐性+20。合計耐性が25以上で雷属性やられ小と大を無効化/雷耐性+15。合計耐性が15以上で雷属性やられ小を無効化/雷耐性-20</t>
   </si>
   <si>
-    <t>狩人</t>
-  </si>
-  <si>
-    <t>ハンター生活</t>
-  </si>
-  <si>
-    <t>こんがり肉を焼きやすくなる。地図が無くてもマップが表示される。釣りで魚が最初の引きで食いつくようになる。釣り餌アイテムの調合が必ず成功する。</t>
+    <t>사냥꾼(狩人)</t>
+  </si>
+  <si>
+    <t>헌터 생활</t>
+  </si>
+  <si>
+    <t>잘 구운 고기로 굽기 쉽게 된다. 지도가 없어도 맵이 표시된다. 낚시에서 물고기가 최초의 당김에  물게 된다. 낚시 미끼 아이템의 조합이 반드시 성공한다.</t>
   </si>
   <si>
     <t>頑強</t>
@@ -1882,7 +1888,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -1912,14 +1918,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1966,7 +1983,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1998,9 +2015,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2032,6 +2067,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2207,12 +2260,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D206"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D20" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="107.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="255.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -2284,7 +2345,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" ht="45">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -2294,7 +2355,7 @@
       <c r="C6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2326,7 +2387,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" ht="75">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -2336,7 +2397,7 @@
       <c r="C9" t="s">
         <v>28</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Skill information translation. (~60)
</commit_message>
<xml_diff>
--- a/skill.xlsx
+++ b/skill.xlsx
@@ -298,7 +298,7 @@
     <t>뇌내성【대】(雷耐性【大】)/뇌내성【소】(雷耐性【小】)/뇌내성 약화(雷耐性弱化)</t>
   </si>
   <si>
-    <t>雷耐性+20。合計耐性が25以上で雷属性やられ小と大を無効化/雷耐性+15。合計耐性が15以上で雷属性やられ小を無効化/雷耐性-20</t>
+    <t>뇌내성+20. 합계내성이 25이상이면 뇌속성 피해 소와 대를 무효화/뇌내성+15. 합계내성이 15이상이면 뇌속성 피해 소 무효화/뇌내성-20</t>
   </si>
   <si>
     <t>사냥꾼(狩人)</t>
@@ -310,253 +310,253 @@
     <t>잘 구운 고기로 굽기 쉽게 된다. 지도가 없어도 맵이 표시된다. 낚시에서 물고기가 최초의 당김에  물게 된다. 낚시 미끼 아이템의 조합이 반드시 성공한다.</t>
   </si>
   <si>
-    <t>頑強</t>
-  </si>
-  <si>
-    <t>鉄壁</t>
-  </si>
-  <si>
-    <t>防御力UP【中】 + 鉄面皮</t>
-  </si>
-  <si>
-    <t>観察眼</t>
-  </si>
-  <si>
-    <t>捕獲の見極め</t>
-  </si>
-  <si>
-    <t>ペイントした時に捕獲できるタイミングでアイコンが白く点滅する</t>
-  </si>
-  <si>
-    <t>貫通弾強化</t>
-  </si>
-  <si>
-    <t>貫通弾・貫通矢UP</t>
-  </si>
-  <si>
-    <t>貫通弾、貫通矢の威力が1.1倍になる</t>
-  </si>
-  <si>
-    <t>貫通弾追加</t>
-  </si>
-  <si>
-    <t>貫通弾全LV追加/貫通弾LV1追加</t>
-  </si>
-  <si>
-    <t>全LVの貫通弾が使えるようになる/LV1貫通弾が使えるようになる</t>
-  </si>
-  <si>
-    <t>寒冷適応</t>
-  </si>
-  <si>
-    <t>北風の狩人</t>
-  </si>
-  <si>
-    <t>寒さ無効と寒い場所で攻撃力15と防御力20上昇。クーラードリンクでさらに攻撃力5アップ</t>
-  </si>
-  <si>
-    <t>祈願</t>
-  </si>
-  <si>
-    <t>祝福</t>
-  </si>
-  <si>
-    <t>体力回復量UP + 精霊の加護</t>
-  </si>
-  <si>
-    <t>気絶</t>
-  </si>
-  <si>
-    <t>気絶無効/気絶確率半減/気絶倍加</t>
-  </si>
-  <si>
-    <t>気絶状態にならなくなる/気絶した際に1/2の確率で気絶効果を無効にする/気絶時間が2倍になり、気絶回復に有効なアナログパッド、ボタンの入力回数が2倍になる</t>
-  </si>
-  <si>
-    <t>気まぐれ</t>
-  </si>
-  <si>
-    <t>神の気まぐれ/精霊の気まぐれ/悪霊の気まぐれ/悪魔の気まぐれ</t>
-  </si>
-  <si>
-    <t>ピッケル系、虫あみ系、笛系、ブーメランが1/2の確率で壊れずに済む/ピッケル系、虫あみ系、笛系、ブーメランが1/3の確率で壊れずに済む/ピッケル系、虫あみ系、笛系、ブーメランが1/4の確率で壊れやすくなる/ピッケル系、虫あみ系、笛系、ブーメランが1/2の確率で壊れやすくなる</t>
-  </si>
-  <si>
-    <t>逆上</t>
-  </si>
-  <si>
-    <t>逆恨み</t>
-  </si>
-  <si>
-    <t>赤ゲージがある間は攻撃力20アップ</t>
-  </si>
-  <si>
-    <t>逆境</t>
-  </si>
-  <si>
-    <t>不屈</t>
-  </si>
-  <si>
-    <t>1回力尽きると攻撃力1.1倍、防御力15%上昇。2回力尽きると攻撃力1.2倍、防御力30%上昇</t>
-  </si>
-  <si>
-    <t>窮地</t>
-  </si>
-  <si>
-    <t>死中に活</t>
-  </si>
-  <si>
-    <t>状態異常時に攻撃力が20上がる</t>
-  </si>
-  <si>
-    <t>狂撃耐性</t>
-  </si>
-  <si>
-    <t>無我の境地</t>
-  </si>
-  <si>
-    <t>狂竜ウイルスを克服しやすくなる。また狂撃化した時に会心率が15%から30%に上がる</t>
-  </si>
-  <si>
-    <t>強撃瓶追加</t>
-  </si>
-  <si>
-    <t>強撃ビン全LV追加/強撃ビンLV1追加</t>
-  </si>
-  <si>
-    <t>全LVの強撃ビンが使えるようになる/強撃ビンLV1の装着が可能になる</t>
-  </si>
-  <si>
-    <t>気力回復</t>
-  </si>
-  <si>
-    <t>スタミナ急速回復/スタミナ回復遅延</t>
-  </si>
-  <si>
-    <t>スタミナの回復速度が2倍になる/スタミナの回復速度が0.75倍に下がる</t>
-  </si>
-  <si>
-    <t>斬れ味</t>
-  </si>
-  <si>
-    <t>業物/なまくら</t>
-  </si>
-  <si>
-    <t>通常攻撃、ガンランスの砲撃、竜撃砲、大剣やチャージアックスのガードによる斬れ味低下が1/2になる。攻撃がはじかれなかった時は1/2で斬れ味が低下しない/斬れ味の消耗が2倍になる</t>
-  </si>
-  <si>
-    <t>金雷公</t>
-  </si>
-  <si>
-    <t>金雷公の魂</t>
-  </si>
-  <si>
-    <t>力の解放+2 + 体術+2</t>
-  </si>
-  <si>
-    <t>銀嶺</t>
-  </si>
-  <si>
-    <t>銀嶺の魂</t>
-  </si>
-  <si>
-    <t>ランナー + 鈍器使い + 通常弾・連射矢UP</t>
-  </si>
-  <si>
-    <t>食いしん坊</t>
-  </si>
-  <si>
-    <t>拾い食い/まんぷく</t>
-  </si>
-  <si>
-    <t>肉アイテム等を食べた時のスタミナが50上昇し、その他の飲食アイテムでもスタミナが25上昇する事がある/肉アイテム等を食べた時のスタミナが50上昇する</t>
+    <t>완강(頑強)</t>
+  </si>
+  <si>
+    <t>철벽(鉄壁)</t>
+  </si>
+  <si>
+    <t>방어력UP【중】(防御力UP【中】) + 철면피(鉄面皮)</t>
+  </si>
+  <si>
+    <t>관찰안(観察眼)</t>
+  </si>
+  <si>
+    <t>포획 판단(捕獲の見極め)</t>
+  </si>
+  <si>
+    <t>페인트 했을 때 포획 가능한 타이밍이 되면 아이콘이 하얗게 점멸한다.</t>
+  </si>
+  <si>
+    <t>관통탄강화(貫通弾強化)</t>
+  </si>
+  <si>
+    <t>관통탄・관통 화살UP(貫通弾・貫通矢UP)</t>
+  </si>
+  <si>
+    <t>관통탄, 광통화살의 위력이 1.1배가 된다.</t>
+  </si>
+  <si>
+    <t>관통탄추가(貫通弾追加)</t>
+  </si>
+  <si>
+    <t>관통탄 전LV 추가(貫通弾全LV追加)/관통탄 LV1 추가(貫通弾LV1追加)</t>
+  </si>
+  <si>
+    <t>전LV의 관통탄을 사용할 수 있게 된다./LV1확산탄을 사용할 수 있게 된다.</t>
+  </si>
+  <si>
+    <t>한랭적응(寒冷適応)</t>
+  </si>
+  <si>
+    <t>북풍의 사냥꾼(北風の狩人)</t>
+  </si>
+  <si>
+    <t>추위 무효와 추운 장소에서 공격력15와 방어력20 상승. 쿨드링크를 마시면 추가로 공격력 5상승</t>
+  </si>
+  <si>
+    <t>기원(祈願)</t>
+  </si>
+  <si>
+    <t>축복(祝福)</t>
+  </si>
+  <si>
+    <t>체력회복량UP(体力回復量UP) + 정령의 가호(精霊の加護)</t>
+  </si>
+  <si>
+    <t>기절(気絶)</t>
+  </si>
+  <si>
+    <t>기절무효(気絶無効)/기절확률반감(気絶確率半減)/기절배가(気絶倍加)</t>
+  </si>
+  <si>
+    <t>기절상태 무효화/기절했을 때 1/2의 확률로 기절효과를 무효화한다./기절시간이 2배가 되고, 기절회복에 유효한 아날로그 패드, 버튼의 입력회수가 2배가 된다.</t>
+  </si>
+  <si>
+    <t>변덕(気まぐれ)</t>
+  </si>
+  <si>
+    <t>신의 변덕(神の気まぐれ)/정령의 변덕(精霊の気まぐれ)/악령의 변덕(悪霊の気まぐれ)/악마의 변덕(悪魔の気まぐれ)</t>
+  </si>
+  <si>
+    <t>곡괭이 계열, 충망 계열, 피리 계열, 부메랑이 1/2의 확률로 부숴지지 않는다./곡괭이 계열, 충망 계열, 피리 계열, 부메랑이 1/3의 확률로 부숴지지 않는다./곡괭이 계열, 충망 계열, 피리 계열, 부메랑이 1/4의 확률로 부숴지지 않는다./곡괭이 계열, 충망 계열, 피리 계열, 부메랑이 1/2의 확률로 부숴지기 쉬워진다.</t>
+  </si>
+  <si>
+    <t>역상(逆上)</t>
+  </si>
+  <si>
+    <t>앙심(逆恨み)</t>
+  </si>
+  <si>
+    <t>체력에 붉은 게이지가 남아있는 동안 공격력20 상승</t>
+  </si>
+  <si>
+    <t>역경(逆境)</t>
+  </si>
+  <si>
+    <t>불굴(不屈)</t>
+  </si>
+  <si>
+    <t>1회 체력이 다하면 공격력1.1배, 방어력15% 상승. 2회 체력이 다하면 공격력1.2배, 방어력30% 상승.</t>
+  </si>
+  <si>
+    <t>궁지(窮地)</t>
+  </si>
+  <si>
+    <t>죽음속에서 삶(死中に活)</t>
+  </si>
+  <si>
+    <t>상태이상 시 공격력20 상승</t>
+  </si>
+  <si>
+    <t>광격내성(狂撃耐性)</t>
+  </si>
+  <si>
+    <t>무아의 경지(無我の境地)</t>
+  </si>
+  <si>
+    <t>광룡 바이러스를 극복하기 쉬워진다. 광격화(광룡 바이러스 극복) 상태일 때 증가하는 회심률이 15%에서 30%로 올라간다.</t>
+  </si>
+  <si>
+    <t>강격병추가(強撃瓶追加)</t>
+  </si>
+  <si>
+    <t>강격병 전LV 추가(強撃ビン全LV追加)/강격병 LV1 추가(強撃ビンLV1追加)</t>
+  </si>
+  <si>
+    <t>전LV의 강격병을 사용할 수 있게된다./강격병LV1의 장착이 가능하게 된다.</t>
+  </si>
+  <si>
+    <t>기력회복(気力回復)</t>
+  </si>
+  <si>
+    <t>스태미너 급속회복(スタミナ急速回復)/스태미너 회복지연(スタミナ回復遅延)</t>
+  </si>
+  <si>
+    <t>스태미너의 회복속도가 2배가 된다./스태미너의 회복속도가 0.75배로 내려간다.</t>
+  </si>
+  <si>
+    <t>예리도(斬れ味)</t>
+  </si>
+  <si>
+    <t>업물(業物)/무딤(なまくら)</t>
+  </si>
+  <si>
+    <t>통상공격, 건랜스 포격, 용격포, 대검이나 차지액스의 가드로 인한 예리도 저하가 1/2이 된다. 공격이 튕겨나가지 않았을 때 1/2의 확률로 예리도가 저하하지 않는다./예리도의 소모가 2배가 된다.</t>
+  </si>
+  <si>
+    <t>금뢰공(金雷公)</t>
+  </si>
+  <si>
+    <t>금뢰공의 혼(金雷公の魂)</t>
+  </si>
+  <si>
+    <t>힘의 해방+2(力の解放+2) + 체술+2(体術+2)</t>
+  </si>
+  <si>
+    <t>은령(銀嶺)</t>
+  </si>
+  <si>
+    <t>은령의 혼(銀嶺の魂)</t>
+  </si>
+  <si>
+    <t>러너(ランナー) + 둔기사용(鈍器使い) + 통상탄・연사 화살UP(通常弾・連射矢UP)</t>
+  </si>
+  <si>
+    <t>먹보(食いしん坊)</t>
+  </si>
+  <si>
+    <t>주워먹기(拾い食い)/만복(まんぷく)</t>
+  </si>
+  <si>
+    <t>고기 아이템 등을 먹었을 때의 스태미너가 50 상승하고, 그 외의 음식 아이템에서도 스태미너가 25 상승하는 경우가 있다./고기 아이템 등을 먹었을 때의 스태미너가 50 상승한다.</t>
   </si>
   <si>
     <t>KO</t>
   </si>
   <si>
-    <t>KO術</t>
-  </si>
-  <si>
-    <t>与えられる気絶値が1.1倍になる。操虫棍の猟虫による打撃には効果無し</t>
-  </si>
-  <si>
-    <t>潔癖</t>
-  </si>
-  <si>
-    <t>舞闘家</t>
-  </si>
-  <si>
-    <t>フルチャージ + 回避距離UP</t>
-  </si>
-  <si>
-    <t>気配</t>
-  </si>
-  <si>
-    <t>隠密/挑発</t>
-  </si>
-  <si>
-    <t>モンスターに狙われにくくなる/モンスターに狙われやすくなる</t>
-  </si>
-  <si>
-    <t>減気攻撃</t>
-  </si>
-  <si>
-    <t>スタミナ奪取</t>
-  </si>
-  <si>
-    <t>打撃属性(抜刀術【力】の斬撃、ボウガンの減気弾、弓の曲射、減気ビンを含む)によるスタミナダメージ値が1.2倍になる</t>
-  </si>
-  <si>
-    <t>減気瓶追加</t>
-  </si>
-  <si>
-    <t>減気ビン追加</t>
-  </si>
-  <si>
-    <t>減気ビンの装着が可能になる</t>
-  </si>
-  <si>
-    <t>剣術</t>
-  </si>
-  <si>
-    <t>心眼/未熟</t>
+    <t>KO술(KO術)</t>
+  </si>
+  <si>
+    <t>가할 수 있는 기절치가 1.1배가 된다. 조충곤의 엽충에 의한 타격에는 효과 없음</t>
+  </si>
+  <si>
+    <t>결벽(潔癖)</t>
+  </si>
+  <si>
+    <t>무투가(舞闘家)</t>
+  </si>
+  <si>
+    <t>풀 차지(フルチャージ) + 회피거리UP(回避距離UP)</t>
+  </si>
+  <si>
+    <t>기척(気配)</t>
+  </si>
+  <si>
+    <t>은밀(隠密)/도발(挑発)</t>
+  </si>
+  <si>
+    <t>몬스터에게 잘 노려지지 않게 된다./몬스터에게 노려지기 쉽게 된다.</t>
+  </si>
+  <si>
+    <t>멸기공격(減気攻撃)</t>
+  </si>
+  <si>
+    <t>스태미너 탈취(スタミナ奪取)</t>
+  </si>
+  <si>
+    <t>타격 속성(발도술【력】의 참격, 보우건의 별기탄, 활의 곡사, 멸기병을 포함)에 의한 스태미너 데미지 수치가 1.2배가 된다.</t>
+  </si>
+  <si>
+    <t>멸기병추가(減気瓶追加)</t>
+  </si>
+  <si>
+    <t>멸기병 추가(減気ビン追加)</t>
+  </si>
+  <si>
+    <t>멸기병의 장착이 가능하게 된다.</t>
+  </si>
+  <si>
+    <t>검술(剣術)</t>
+  </si>
+  <si>
+    <t>심안(心眼)/미숙(未熟)</t>
   </si>
   <si>
     <t>攻撃がはじかれる判定になってもはじかれモーションを取らなくなる/通常弾かれない場合でも1/3の確率で弾かれる</t>
   </si>
   <si>
-    <t>研磨術</t>
-  </si>
-  <si>
-    <t>剛刃研磨</t>
+    <t>연마술(研磨術)</t>
+  </si>
+  <si>
+    <t>강인연마(剛刃研磨)</t>
   </si>
   <si>
     <t>砥石やキレアジを使うと1分間斬れ味が減らなくなる。ガンナーの場合でも砥石が使えて、1分間、適正距離での射撃で攻撃倍率が1.75倍になる</t>
   </si>
   <si>
-    <t>広域</t>
-  </si>
-  <si>
-    <t>広域化+2/広域化+1</t>
+    <t>광역(広域)</t>
+  </si>
+  <si>
+    <t>광역화+2(広域化+2)/광역화+1(広域化+1)</t>
   </si>
   <si>
     <t>薬草、回復薬、解毒薬、忍耐の種、怪力の種、ウチケシの実の効果が同じエリア内にいる他のハンター、オトモにも効果が発動/薬草、回復薬、解毒薬、忍耐の種、怪力の種、ウチケシの実の効果が同じエリア内にいる他のハンター、オトモにも効果が発動。ただし解毒薬以外は効果が半分になる</t>
   </si>
   <si>
-    <t>効果持続</t>
-  </si>
-  <si>
-    <t>アイテム使用強化/アイテム使用弱化</t>
+    <t>효과지속(効果持続)</t>
+  </si>
+  <si>
+    <t>아이템 사용 강화(アイテム使用強化)/아이템 사용 약화(アイテム使用弱化)</t>
   </si>
   <si>
     <t>薬、ドリンク、種、丸薬などのアイテムやスキル「剛刃研磨」の効果持続時間が1.5倍になる/薬、ドリンク、種、丸薬などのアイテムやスキル「剛刃研磨」の効果持続時間が2/3になる</t>
   </si>
   <si>
-    <t>攻撃</t>
-  </si>
-  <si>
-    <t>攻撃力UP【大】/攻撃力UP【中】/攻撃力UP【小】/攻撃力DOWN【小】/攻撃力DOWN【中】/攻撃力DOWN【大】</t>
+    <t>공격(攻撃)</t>
+  </si>
+  <si>
+    <t>공격력UP【대】(攻撃力UP【大】)/공격력UP【중】(攻撃力UP【中】)/공격력UP【소】(攻撃力UP【小】)/공격력DOWN【소】(攻撃力DOWN【小】)/공격력DOWN【중】(攻撃力DOWN【中】)/공격력DOWN【대】(攻撃力DOWN【大】)</t>
   </si>
   <si>
     <t>20/15/10/-10/-15/-20</t>
@@ -565,22 +565,22 @@
     <t>攻撃力+20/攻撃力+15/攻撃力+10/攻撃力-5/攻撃力-10/攻撃力-15</t>
   </si>
   <si>
-    <t>剛撃</t>
-  </si>
-  <si>
-    <t>無慈悲</t>
+    <t>강격(剛撃)</t>
+  </si>
+  <si>
+    <t>무자비(無慈悲)</t>
   </si>
   <si>
     <t>見切り+2 + 弱点特効</t>
   </si>
   <si>
-    <t>高速設置</t>
-  </si>
-  <si>
-    <t>罠師</t>
-  </si>
-  <si>
-    <t>罠アイテム、肉アイテム、爆弾(小タル爆弾と打ち上げタル爆弾以外)の設置時間が短くなる。さらに罠アイテムと肉アイテムの調合成功率が100％になる</t>
+    <t>고속설치(高速設置)</t>
+  </si>
+  <si>
+    <t>함정꾼(罠師)</t>
+  </si>
+  <si>
+    <t>함정 아이템, 고기(설치용) 아이템、폭탄(작은 통 폭탄과 발사 통 폭탄 이외)의 설치시간이 짧아진다. 함정 아이템과 고기 아이템의 조합성공률이 100%가 된다.</t>
   </si>
   <si>
     <t>強欲</t>
@@ -2263,8 +2263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D20" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Skill information translation. (~104)
</commit_message>
<xml_diff>
--- a/skill.xlsx
+++ b/skill.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="621">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="620">
   <si>
     <t>skillType</t>
   </si>
@@ -523,7 +523,7 @@
     <t>심안(心眼)/미숙(未熟)</t>
   </si>
   <si>
-    <t>攻撃がはじかれる判定になってもはじかれモーションを取らなくなる/通常弾かれない場合でも1/3の確率で弾かれる</t>
+    <t>공격이 튕겨나가는 판정이 되어도 튕김 모션을 취하지 않게 된다./통상 튕겨나가지 않는 경우에도 1/3의 확률로 튕겨나간다.</t>
   </si>
   <si>
     <t>연마술(研磨術)</t>
@@ -532,7 +532,7 @@
     <t>강인연마(剛刃研磨)</t>
   </si>
   <si>
-    <t>砥石やキレアジを使うと1分間斬れ味が減らなくなる。ガンナーの場合でも砥石が使えて、1分間、適正距離での射撃で攻撃倍率が1.75倍になる</t>
+    <t>숫돌이나 예리어를 사용하면 1분간 예리도가 줄어들지 않게 된다. 거너의 경우에도 숫돌을 사용 가능하게 되며, 1분간 적정거리 사격에서의 공격 배율이 1.75배가 된다.</t>
   </si>
   <si>
     <t>광역(広域)</t>
@@ -541,7 +541,7 @@
     <t>광역화+2(広域化+2)/광역화+1(広域化+1)</t>
   </si>
   <si>
-    <t>薬草、回復薬、解毒薬、忍耐の種、怪力の種、ウチケシの実の効果が同じエリア内にいる他のハンター、オトモにも効果が発動/薬草、回復薬、解毒薬、忍耐の種、怪力の種、ウチケシの実の効果が同じエリア内にいる他のハンター、オトモにも効果が発動。ただし解毒薬以外は効果が半分になる</t>
+    <t>약초, 회복약, 해독약, 인내의 씨앗, 괴력의 씨앗, 지움 열매의 효과가 같은 에어리어 내에 있는 다른 헌터, 오토모에게도 효과가 발동/약초, 회복약, 해독약, 인내의 씨앗, 괴력의 씨앗, 지움 열매의 효과가 같은 에어리어 내에 있는 다른 헌터, 오토모에게도 효과가 발동, 단 해독약 이외는 효과가 반감한다.</t>
   </si>
   <si>
     <t>효과지속(効果持続)</t>
@@ -550,7 +550,7 @@
     <t>아이템 사용 강화(アイテム使用強化)/아이템 사용 약화(アイテム使用弱化)</t>
   </si>
   <si>
-    <t>薬、ドリンク、種、丸薬などのアイテムやスキル「剛刃研磨」の効果持続時間が1.5倍になる/薬、ドリンク、種、丸薬などのアイテムやスキル「剛刃研磨」の効果持続時間が2/3になる</t>
+    <t>약, 드링크, 씨앗, 환약 등의 아이템이나 스킬 「강인연마」의 효과 지속시간이 1.5배가 된다./약, 드링크, 씨앗, 환약 등의 아이템이나 스킬 「강인연마」의 효과 지속시간이 2/3이 된다.</t>
   </si>
   <si>
     <t>공격(攻撃)</t>
@@ -562,7 +562,7 @@
     <t>20/15/10/-10/-15/-20</t>
   </si>
   <si>
-    <t>攻撃力+20/攻撃力+15/攻撃力+10/攻撃力-5/攻撃力-10/攻撃力-15</t>
+    <t>공격력+20(攻撃力+20)/공격력+15(攻撃力+15)/공격력+10(攻撃力+10)/공격력-5(攻撃力-5)/공격력-10(攻撃力-10)/공격력-15(攻撃力-15)</t>
   </si>
   <si>
     <t>강격(剛撃)</t>
@@ -571,7 +571,7 @@
     <t>무자비(無慈悲)</t>
   </si>
   <si>
-    <t>見切り+2 + 弱点特効</t>
+    <t>간파+2(見切り+2) + 약점특효(弱点特効)</t>
   </si>
   <si>
     <t>고속설치(高速設置)</t>
@@ -583,397 +583,394 @@
     <t>함정 아이템, 고기(설치용) 아이템、폭탄(작은 통 폭탄과 발사 통 폭탄 이외)의 설치시간이 짧아진다. 함정 아이템과 고기 아이템의 조합성공률이 100%가 된다.</t>
   </si>
   <si>
-    <t>強欲</t>
-  </si>
-  <si>
-    <t>増収</t>
-  </si>
-  <si>
-    <t>強運 + 捕獲達人</t>
-  </si>
-  <si>
-    <t>号令</t>
-  </si>
-  <si>
-    <t>オトモへの号令</t>
-  </si>
-  <si>
-    <t>オトモが休息している状態でアクションかけごえを実行すると、オトモの体力が満タンになる。使用後から10分間は再使用できない。</t>
-  </si>
-  <si>
-    <t>剛腕</t>
-  </si>
-  <si>
-    <t>痛打</t>
-  </si>
-  <si>
-    <t>スタミナ奪取 + KO術</t>
-  </si>
-  <si>
-    <t>氷属性攻撃</t>
-  </si>
-  <si>
-    <t>氷属性攻撃強化+2/氷属性攻撃強化+1/氷属性攻撃弱化</t>
-  </si>
-  <si>
-    <t>氷属性の攻撃が1.1倍+6になる/氷属性の攻撃が1.05倍+4になる/氷属性の攻撃が0.75倍になる</t>
-  </si>
-  <si>
-    <t>氷耐性</t>
-  </si>
-  <si>
-    <t>氷耐性【大】/氷耐性【小】/氷耐性弱化</t>
-  </si>
-  <si>
-    <t>氷耐性+20。合計耐性が25以上で氷属性やられ小と大を無効化/氷耐性+15。合計耐性が15以上で氷属性やられ小を無効化/氷耐性-20</t>
-  </si>
-  <si>
-    <t>黒炎王</t>
-  </si>
-  <si>
-    <t>黒炎王の魂</t>
-  </si>
-  <si>
-    <t>風圧【大】無効 + 攻撃力UP【大】</t>
-  </si>
-  <si>
-    <t>ココット</t>
-  </si>
-  <si>
-    <t>ココットの心</t>
-  </si>
-  <si>
-    <t>雷耐性【小】 + 精霊の気まぐれ</t>
-  </si>
-  <si>
-    <t>護石王</t>
-  </si>
-  <si>
-    <t>お守りハンター/お守り収集</t>
-  </si>
-  <si>
-    <t>採集時にお守りが30%の確率で2つ入手できるようになる/採集時にお守りが20%の確率で2つ入手できるようになる</t>
-  </si>
-  <si>
-    <t>護石強化</t>
-  </si>
-  <si>
-    <t>護石系統倍加</t>
-  </si>
-  <si>
-    <t>装備している護石のスキルポイントが倍になる。</t>
-  </si>
-  <si>
-    <t>護石収集</t>
-  </si>
-  <si>
-    <t>お守りマニア</t>
-  </si>
-  <si>
-    <t>お守りハンター + 採取+1</t>
-  </si>
-  <si>
-    <t>根性</t>
-  </si>
-  <si>
-    <t>体力が64以上残っている場合、それ以上の攻撃を受けても力尽きずギリギリで踏みとどまる。一回発動すると効果が失われるが、力尽きると再度効果が発生する</t>
-  </si>
-  <si>
-    <t>細菌学</t>
-  </si>
-  <si>
-    <t>バイオドクター/細菌研究家</t>
-  </si>
-  <si>
-    <t>こやし玉を当てたモンスターが必ずエリア移動する。肥やし玉の調合が必ず成功する。一部アイテム使用不可、爆破やられにならなくなる。狂竜症発症時間が0.8倍に緩和される/こやし玉を当てたモンスターが必ずエリア移動する。肥やし玉の調合が必ず成功する。一部アイテム使用不可、爆破やられにならなくなる</t>
-  </si>
-  <si>
-    <t>採取</t>
-  </si>
-  <si>
-    <t>採取+2/採取+1/採取-1</t>
-  </si>
-  <si>
-    <t>アイテムの次回も採取できる確率が通常の25/32から29/32になる。/アイテムの次回も採取できる確率が通常の25/32から27/32になる。/アイテムの次回も採取できる確率が通常の25/32から21/32になる。</t>
-  </si>
-  <si>
-    <t>采配</t>
-  </si>
-  <si>
-    <t>オトモへの采配</t>
-  </si>
-  <si>
-    <t>オトモの攻撃力と防御力が1.1倍になる</t>
-  </si>
-  <si>
-    <t>斬術</t>
-  </si>
-  <si>
-    <t>心剣一体</t>
-  </si>
-  <si>
-    <t>心眼 + 業物</t>
-  </si>
-  <si>
-    <t>散弾強化</t>
-  </si>
-  <si>
-    <t>散弾・拡散矢UP</t>
-  </si>
-  <si>
-    <t>散弾の威力が1.2倍になる。拡散矢の威力が1.3倍になる</t>
-  </si>
-  <si>
-    <t>散弾追加</t>
-  </si>
-  <si>
-    <t>散弾全LV追加/散弾LV1追加</t>
-  </si>
-  <si>
-    <t>全LVの散弾が使えるようになる/LV1散弾が使えるようになる</t>
-  </si>
-  <si>
-    <t>紫毒姫</t>
-  </si>
-  <si>
-    <t>紫毒姫の魂</t>
-  </si>
-  <si>
-    <t>状態異常攻撃+2 + 広域化+2</t>
-  </si>
-  <si>
-    <t>射手</t>
-  </si>
-  <si>
-    <t>剛弾</t>
-  </si>
-  <si>
-    <t>通常弾・連射矢UP + 貫通弾・貫通矢UP + 散弾・拡散矢UP</t>
-  </si>
-  <si>
-    <t>射法</t>
-  </si>
-  <si>
-    <t>弾導強化</t>
-  </si>
-  <si>
-    <t>通常弾、貫通弾、矢の適正距離の範囲が広がる</t>
-  </si>
-  <si>
-    <t>重撃</t>
-  </si>
-  <si>
-    <t>破壊王</t>
-  </si>
-  <si>
-    <t>部位破壊の蓄積値が1.3倍になり、モンスターがひるみやすくなる。部位耐久値へのダメージが増えるだけで体力を減らすダメージは増えない。部位破壊後は効果が無い</t>
-  </si>
-  <si>
-    <t>重撃弾強化</t>
-  </si>
-  <si>
-    <t>重撃弾・重射矢UP</t>
-  </si>
-  <si>
-    <t>重撃弾、重射矢の攻撃力が1.1倍になる</t>
-  </si>
-  <si>
-    <t>状態耐性</t>
-  </si>
-  <si>
-    <t>護法</t>
-  </si>
-  <si>
-    <t>毒耐性 + 麻痺無効 + 睡眠無効 + 気絶無効</t>
-  </si>
-  <si>
-    <t>職工</t>
-  </si>
-  <si>
-    <t>トラップマスター</t>
-  </si>
-  <si>
-    <t>ボマー + 罠師</t>
-  </si>
-  <si>
-    <t>食事</t>
-  </si>
-  <si>
-    <t>早食い+2/早食い+1/スローライフ</t>
-  </si>
-  <si>
-    <t>肉系を食べる速度が1.8倍になり、アイテムを飲んだ時の動作が1.7倍になる/肉系を食べる速度が1.7倍になる/肉系を食べる速度が遅くなる</t>
-  </si>
-  <si>
-    <t>食欲</t>
-  </si>
-  <si>
-    <t>グルメ</t>
-  </si>
-  <si>
-    <t>早食い+2 + お肉大好き + キノコ大好き</t>
-  </si>
-  <si>
-    <t>白疾風</t>
-  </si>
-  <si>
-    <t>白疾風の魂</t>
-  </si>
-  <si>
-    <t>回避性能+2 + 見切り+3</t>
-  </si>
-  <si>
-    <t>真・荒鉤爪</t>
-  </si>
-  <si>
-    <t>真・荒鉤爪の魂</t>
-  </si>
-  <si>
-    <t>早食い+2 + 高級耳栓 + ＳＰ時間延長</t>
-  </si>
-  <si>
-    <t>真・岩穿</t>
-  </si>
-  <si>
-    <t>真・岩穿の魂</t>
-  </si>
-  <si>
-    <t>火事場力+2 + 拾い食い + 砲術王</t>
-  </si>
-  <si>
-    <t>真・鏖魔</t>
-  </si>
-  <si>
-    <t>真・鏖魔の魂</t>
-  </si>
-  <si>
-    <t>攻撃力UP【大】 + 回避性能+2 + 明鏡止水</t>
-  </si>
-  <si>
-    <t>真・大雪主</t>
-  </si>
-  <si>
-    <t>真・大雪主の魂</t>
-  </si>
-  <si>
-    <t>回避距離UP + 乗り名人 + スタミナ急速回復</t>
-  </si>
-  <si>
-    <t>真・朧隠</t>
-  </si>
-  <si>
-    <t>真・朧隠の魂</t>
-  </si>
-  <si>
-    <t>高級耳栓 + 装填速度+3 + 心剣一体 + 罠師</t>
-  </si>
-  <si>
-    <t>真・金雷公</t>
-  </si>
-  <si>
-    <t>真・金雷公の魂</t>
-  </si>
-  <si>
-    <t>力の解放+2 + 体術+2 + 集中</t>
-  </si>
-  <si>
-    <t>真・銀嶺</t>
-  </si>
-  <si>
-    <t>真・銀嶺の魂</t>
-  </si>
-  <si>
-    <t>ランナー + 鈍器使い + 通常弾・連射矢UP + 攻撃力UP【中】</t>
-  </si>
-  <si>
-    <t>真・黒炎王</t>
-  </si>
-  <si>
-    <t>真・黒炎王の魂</t>
-  </si>
-  <si>
-    <t>風圧【大】無効 + 攻撃力UP【大】 + 火事場力+1</t>
-  </si>
-  <si>
-    <t>真・紫毒姫</t>
-  </si>
-  <si>
-    <t>真・紫毒姫の魂</t>
-  </si>
-  <si>
-    <t>状態異常攻撃+2 + 広域化+2 + 薬草超強化</t>
-  </si>
-  <si>
-    <t>真・白疾風</t>
-  </si>
-  <si>
-    <t>真・白疾風の魂</t>
-  </si>
-  <si>
-    <t>回避性能+2 + 見切り+3 + 隠密</t>
-  </si>
-  <si>
-    <t>真・燼滅刃</t>
-  </si>
-  <si>
-    <t>真・燼滅刃の魂</t>
-  </si>
-  <si>
-    <t>斬れ味レベル+2 + ボマー + 弾導強化 + 砥石使用高速化</t>
-  </si>
-  <si>
-    <t>真・青電主</t>
-  </si>
-  <si>
-    <t>真・青電主の魂</t>
-  </si>
-  <si>
-    <t>超会心 + 連発数+1 + 斬れ味レベル+1 + 虎視眈々</t>
-  </si>
-  <si>
-    <t>真・隻眼</t>
-  </si>
-  <si>
-    <t>真・隻眼の魂</t>
-  </si>
-  <si>
-    <t>気絶無効 + 挑戦者+2 + 不屈</t>
-  </si>
-  <si>
-    <t>真・宝纏</t>
-  </si>
-  <si>
-    <t>真・宝纏の魂</t>
-  </si>
-  <si>
-    <t>お守りハンター + 英雄の護り + 腹減り無効</t>
-  </si>
-  <si>
-    <t>真・天眼</t>
-  </si>
-  <si>
-    <t>真・天眼の魂</t>
-  </si>
-  <si>
-    <t>見切り+3 + 挑戦者+2</t>
-  </si>
-  <si>
-    <t>真・紅兜</t>
-  </si>
-  <si>
-    <t>真・紅兜の魂</t>
-  </si>
-  <si>
-    <t>逆恨み + 集中 + ランナー</t>
-  </si>
-  <si>
-    <t>真・矛砕</t>
-  </si>
-  <si>
-    <t>真・矛砕の魂</t>
-  </si>
-  <si>
-    <t>業物 + 反動軽減+2 + 精霊の加護 + 体術+1</t>
+    <t>강욕(強欲)</t>
+  </si>
+  <si>
+    <t>증수(増収)</t>
+  </si>
+  <si>
+    <t>강운(強運) + 포획달인(捕獲達人)</t>
+  </si>
+  <si>
+    <t>호령(号令)</t>
+  </si>
+  <si>
+    <t>오토모 호령(オトモへの号令)</t>
+  </si>
+  <si>
+    <t>오토모가 휴식하고 있는 상태에서 액션 구호(かけごえ)를 실행하면, 오토모의 체력이 최대로 회복된다. 사용 후로부터 10분간 재사용 불가능</t>
+  </si>
+  <si>
+    <t>강완(剛腕)</t>
+  </si>
+  <si>
+    <t>통타(痛打)</t>
+  </si>
+  <si>
+    <t>스태미너 탈취(スタミナ奪取) + KO술(KO術)</t>
+  </si>
+  <si>
+    <t>빙속성 공격(氷属性攻撃)</t>
+  </si>
+  <si>
+    <t>빙속성 공격강화+2(氷属性攻撃強化+2)/빙속성 공격강화+1(氷属性攻撃強化+1)/빙속성 공격약화(氷属性攻撃弱化)</t>
+  </si>
+  <si>
+    <t>빙속성의 공격이 1.1배+6이 된다./빙속성의 공격이 1.05배+4가 된다./빙속성의 공격이 0.75배가 된다.</t>
+  </si>
+  <si>
+    <t>빙내성(氷耐性)</t>
+  </si>
+  <si>
+    <t>빙내성【대】(氷耐性【大】)/빙내성【소】(氷耐性【小】)/빙내성 약화(氷耐性弱化)</t>
+  </si>
+  <si>
+    <t>빙내성+20. 합계내성이 25이상이면 빙속성 피해 소와 대를 무효화/빙내성+15. 합계내성이 15이상이면 빙속성 피해 소 무효화/빙내성-20</t>
+  </si>
+  <si>
+    <t>흑염왕(黒炎王)</t>
+  </si>
+  <si>
+    <t>흑염왕의 혼(黒炎王の魂)</t>
+  </si>
+  <si>
+    <t>풍압【대】 무효(風圧【大】無効) + 공격력UP【대】(攻撃力UP【大】) + 화사장력+1(火事場力+1)</t>
+  </si>
+  <si>
+    <t>코코트(ココット)</t>
+  </si>
+  <si>
+    <t>코코트의 마음(ココットの心)</t>
+  </si>
+  <si>
+    <t>뇌내성【소】(雷耐性【小】) + 정령의 변덕(精霊の気まぐれ)</t>
+  </si>
+  <si>
+    <t>호석왕(護石王)</t>
+  </si>
+  <si>
+    <t>부적 헌터(お守りハンター)/부적 수집(お守り収集)</t>
+  </si>
+  <si>
+    <t>채집 시에 부적이 30% 확률로 2개 입수 가능하게 된다./채집 시에 부적이 20% 확률로 2개 입수 가능하게 된다.</t>
+  </si>
+  <si>
+    <t>호석강화(護石強化)</t>
+  </si>
+  <si>
+    <t>호석계통배가(護石系統倍加)</t>
+  </si>
+  <si>
+    <t>장비하고 있는 호석의 스킬포인트가 배가 된다.</t>
+  </si>
+  <si>
+    <t>호석수집(護石収集)</t>
+  </si>
+  <si>
+    <t>부적 매니아(お守りマニア)</t>
+  </si>
+  <si>
+    <t>부적 헌터(お守りハンター) + 채취+1(採取+1)</t>
+  </si>
+  <si>
+    <t>근성(根性)</t>
+  </si>
+  <si>
+    <t>체력이 64이상 남아있을 경우 그 이상의 공격을 받아도 사망하지 않고 1의 체력으로 버틴다. . 1회 발동하면 효과를 잃어버리나 사망하면 다시 효과가 발생한다.</t>
+  </si>
+  <si>
+    <t>세균학(細菌学)</t>
+  </si>
+  <si>
+    <t>바이오 닥터(バイオドクター)/세균 연구가(細菌研究家)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">비료옥을 맞춘 몬스터가 반드시 에어리어를 이동한다. 비료옥의 조합이 반드시 성공한다. 일부 아이템 사용불가, 폭파 피해 상태가 되지 않는다. 광룡증 발증 시간이 0.8배로 완화된다./비료옥을 맞춘 몬스터가 반드시 에어리어를 이동한다. 비료옥의 조합이 반드시 성공한다. 일부 아이템 사용불가, 폭파 피해 상태가 되지 않는다. </t>
+  </si>
+  <si>
+    <t>채취(採取)</t>
+  </si>
+  <si>
+    <t>채취+2(採取+2)/채취+1(採取+1)/채취-1(採取-1)</t>
+  </si>
+  <si>
+    <t>아이템을 다음회도 채취할 수 있는 확률이 통상의 25/32에서 29/32가 된다./아이템을 다음회도 채취할 수 있는 확률이 통상의 25/32에서 27/32가 된다./아이템을 다음회도 채취할 수 있는 확률이 통상의 25/32에서 21/32가 된다.</t>
+  </si>
+  <si>
+    <t>지휘(采配)</t>
+  </si>
+  <si>
+    <t>오토모 지휘(オトモへの采配)</t>
+  </si>
+  <si>
+    <t>오토모의 공격력과 방어력이 1.1배가 된다.</t>
+  </si>
+  <si>
+    <t>참술(斬術)</t>
+  </si>
+  <si>
+    <t>심검일체(心剣一体)</t>
+  </si>
+  <si>
+    <t>심안(心眼) + 업물(業物)</t>
+  </si>
+  <si>
+    <t>산탄강화(散弾強化)</t>
+  </si>
+  <si>
+    <t>산탄・확산 화살UP(散弾・拡散矢UP)</t>
+  </si>
+  <si>
+    <t>산탄의 위력이 1.2배가 된다. 확산 화살의 위력이 1.3배가 된다.</t>
+  </si>
+  <si>
+    <t>산탄추가(散弾追加)</t>
+  </si>
+  <si>
+    <t>산탄 전LV 추가(散弾全LV追加)/산탄 LV1 추가(散弾LV1追加)</t>
+  </si>
+  <si>
+    <t>전LV의 산탄을 사용할 수 있게 된다./LV1산탄을 사용할 수 있게 된다.</t>
+  </si>
+  <si>
+    <t>자독희(紫毒姫)</t>
+  </si>
+  <si>
+    <t>자독희의 혼(紫毒姫の魂)</t>
+  </si>
+  <si>
+    <t>상태이상공격+2(状態異常攻撃+2) + 광역화+2(広域化+2)</t>
+  </si>
+  <si>
+    <t>사수(射手)</t>
+  </si>
+  <si>
+    <t>강탄(剛弾)</t>
+  </si>
+  <si>
+    <t>통상탄・연사 화살UP(通常弾・連射矢UP) + 관통탄・관통 화살UP(貫通弾・貫通矢UP) + 산탄・확산 화살UP(散弾・拡散矢UP)</t>
+  </si>
+  <si>
+    <t>사법(射法)</t>
+  </si>
+  <si>
+    <t>탄도강화(弾導強化)</t>
+  </si>
+  <si>
+    <t>통상탄, 관통탄, 화살의 적정거리 범위가 넓어진다.</t>
+  </si>
+  <si>
+    <t>중격(重撃)</t>
+  </si>
+  <si>
+    <t>파괴왕(破壊王)</t>
+  </si>
+  <si>
+    <t>부위 파괴의 축적치가 1.3배가 되고 몬스터가 기죽기 쉽게 된다. 부위 내구치에 가하는 데미지가 늘어나는 것일 뿐이고 체력을 줄이는 데미지는 늘어나지 않는다. 부위 파괴 후에는 효과 없음</t>
+  </si>
+  <si>
+    <t>중격탄 강화(重撃弾強化)</t>
+  </si>
+  <si>
+    <t>중격탄・중사 화살UP(重撃弾・重射矢UP)</t>
+  </si>
+  <si>
+    <t>중격탄, 중사 화살의 공격력이 1.1배가 된다.</t>
+  </si>
+  <si>
+    <t>상태내성(状態耐性)</t>
+  </si>
+  <si>
+    <t>호법(護法)</t>
+  </si>
+  <si>
+    <t>독내성(毒耐性) + 마비무효(麻痺無効) + 수면무효(睡眠無効) + 기절무효(気絶無効)</t>
+  </si>
+  <si>
+    <t>직공(職工)</t>
+  </si>
+  <si>
+    <t>트랩 마스터(トラップマスター)</t>
+  </si>
+  <si>
+    <t>보머(ボマー) + 함정꾼(罠師)</t>
+  </si>
+  <si>
+    <t>식사(食事)</t>
+  </si>
+  <si>
+    <t>속식+2(早食い+2)/속식+1(早食い+1)/슬로우 라이프(スローライフ)</t>
+  </si>
+  <si>
+    <t>고기 계열을 먹는 속도가 1.8배가 되고, 아이템을 마시는 속도가 1.7배가 된다./고기 계열을 먹는 속도가 1.7배가 된다./고기 계열을 먹는 속도가 느려진다.</t>
+  </si>
+  <si>
+    <t>식욕(食欲)</t>
+  </si>
+  <si>
+    <t>미식가(グルメ)</t>
+  </si>
+  <si>
+    <t>속식+2(早食い+2) + 고기 애호가(お肉大好き) + 버섯 애호가(キノコ大好き)</t>
+  </si>
+  <si>
+    <t>백질풍(白疾風)</t>
+  </si>
+  <si>
+    <t>백질풍의 혼(白疾風の魂)</t>
+  </si>
+  <si>
+    <t>회피성능+2(回避性能+2) + 간파+3(見切り+3)</t>
+  </si>
+  <si>
+    <t>진・황구조(真・荒鉤爪)</t>
+  </si>
+  <si>
+    <t>진・황구조의 혼(真・荒鉤爪の魂)</t>
+  </si>
+  <si>
+    <t>속식+2(早食い+2) + 고급 귀마개(高級耳栓) + SP시간연장(ＳＰ時間延長)</t>
+  </si>
+  <si>
+    <t>진・암천(真・岩穿)</t>
+  </si>
+  <si>
+    <t>진・암천의 혼(真・岩穿の魂)</t>
+  </si>
+  <si>
+    <t>화사장력+2(火事場力+2) + 주워먹기(拾い食い) + 포술왕(砲術王)</t>
+  </si>
+  <si>
+    <t>진・오마(真・鏖魔)</t>
+  </si>
+  <si>
+    <t>진・오마의 혼(真・鏖魔の魂)</t>
+  </si>
+  <si>
+    <t>공격력UP【대】(攻撃力UP【大】) + 회피성능+2(回避性能+2) + 명경지수(明鏡止水)</t>
+  </si>
+  <si>
+    <t>진・대설주(真・大雪主)</t>
+  </si>
+  <si>
+    <t>진・대설주의 혼(真・大雪主の魂)</t>
+  </si>
+  <si>
+    <t>회피거리UP(回避距離UP) + 탑승 명인(乗り名人) + 스태미너 급속회복(スタミナ急速回復)</t>
+  </si>
+  <si>
+    <t>진・농은(真・朧隠)</t>
+  </si>
+  <si>
+    <t>진・농은의 혼(真・朧隠の魂)</t>
+  </si>
+  <si>
+    <t>고급 귀마개(高級耳栓) + 장전속도+3(装填速度+3) + 심검일체(心剣一体) + 함정꾼(罠師)</t>
+  </si>
+  <si>
+    <t>진・금뢰공(真・金雷公)</t>
+  </si>
+  <si>
+    <t>진・금뢰공의 혼(真・金雷公の魂)</t>
+  </si>
+  <si>
+    <t>힘의 해방+2(力の解放+2) + 체술+2(体術+2) + 집중(集中)</t>
+  </si>
+  <si>
+    <t>진・은령(真・銀嶺)</t>
+  </si>
+  <si>
+    <t>진・은령의 혼(真・銀嶺の魂)</t>
+  </si>
+  <si>
+    <t>러너(ランナー) + 둔기 사용(鈍器使い) + 통상탄・연사 화살UP(通常弾・連射矢UP) + 공격력UP【중】(攻撃力UP【中】)</t>
+  </si>
+  <si>
+    <t>진・흑염왕(真・黒炎王)</t>
+  </si>
+  <si>
+    <t>진・흑염왕의 혼(真・黒炎王の魂)</t>
+  </si>
+  <si>
+    <t>진・자독희(真・紫毒姫)</t>
+  </si>
+  <si>
+    <t>진・자독희의 혼(真・紫毒姫の魂)</t>
+  </si>
+  <si>
+    <t>상태이상공격+2(状態異常攻撃+2) + 광역화+2(広域化+2) + 약초 초 강화(薬草超強化)</t>
+  </si>
+  <si>
+    <t>진・백질풍(真・白疾風)</t>
+  </si>
+  <si>
+    <t>진・백질풍의 혼(真・白疾風の魂)</t>
+  </si>
+  <si>
+    <t>회피성능+2(回避性能+2) + 간파+3(見切り+3) + 은밀(隠密)</t>
+  </si>
+  <si>
+    <t>진・신멸인(真・燼滅刃)</t>
+  </si>
+  <si>
+    <t>진・신멸인의 혼(真・燼滅刃の魂)</t>
+  </si>
+  <si>
+    <t>예리도 레벨+2(斬れ味レベル+2) + 보머(ボマー) + 탄도강화(弾導強化) + 숫돌 사용 고속화(砥石使用高速化)</t>
+  </si>
+  <si>
+    <t>진・청전주(真・青電主)</t>
+  </si>
+  <si>
+    <t>진・청전주의 혼(真・青電主の魂)</t>
+  </si>
+  <si>
+    <t>초회심(超会心) + 연발수+1(連発数+1) + 예리도 레벨+1(斬れ味レベル+1) + 호시탐탐(虎視眈々)</t>
+  </si>
+  <si>
+    <t>진・척안(真・隻眼)</t>
+  </si>
+  <si>
+    <t>진・척안의 혼(真・隻眼の魂)</t>
+  </si>
+  <si>
+    <t>기절무효(気絶無効) + 도전자+2(挑戦者+2) + 불굴(不屈)</t>
+  </si>
+  <si>
+    <t>진・보전(真・宝纏)</t>
+  </si>
+  <si>
+    <t>진・보전의 혼(真・宝纏の魂)</t>
+  </si>
+  <si>
+    <t>부적 헌터(お守りハンター) + 영웅의 수호(英雄の護り) + 배고픔 무효(腹減り無効)</t>
+  </si>
+  <si>
+    <t>진・천안(真・天眼)</t>
+  </si>
+  <si>
+    <t>진・천안의 혼(真・天眼の魂)</t>
+  </si>
+  <si>
+    <t>간파+3(見切り+3) + 도전자+2(挑戦者+2)</t>
+  </si>
+  <si>
+    <t>진・홍두(真・紅兜)</t>
+  </si>
+  <si>
+    <t>진・홍두의 혼(真・紅兜の魂)</t>
+  </si>
+  <si>
+    <t>앙심(逆恨み) + 집중(集中) + 러너(ランナー)</t>
+  </si>
+  <si>
+    <t>진・모쇄(真・矛砕)</t>
+  </si>
+  <si>
+    <t>진・모쇄의 혼(真・矛砕の魂)</t>
+  </si>
+  <si>
+    <t>업물(業物) + 반동경감+2(反動軽減+2) + 정령의 가호(精霊の加護) + 체술+1(体術+1)</t>
   </si>
   <si>
     <t>燼滅刃</t>
@@ -2263,8 +2260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="C86" workbookViewId="0">
+      <selection activeCell="D103" sqref="D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3602,1561 +3599,1561 @@
         <v>6</v>
       </c>
       <c r="D95" t="s">
-        <v>290</v>
+        <v>204</v>
       </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" t="s">
+        <v>290</v>
+      </c>
+      <c r="B96" t="s">
         <v>291</v>
       </c>
-      <c r="B96" t="s">
+      <c r="C96" t="s">
+        <v>6</v>
+      </c>
+      <c r="D96" t="s">
         <v>292</v>
-      </c>
-      <c r="C96" t="s">
-        <v>6</v>
-      </c>
-      <c r="D96" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" t="s">
+        <v>293</v>
+      </c>
+      <c r="B97" t="s">
         <v>294</v>
       </c>
-      <c r="B97" t="s">
+      <c r="C97" t="s">
+        <v>6</v>
+      </c>
+      <c r="D97" t="s">
         <v>295</v>
-      </c>
-      <c r="C97" t="s">
-        <v>6</v>
-      </c>
-      <c r="D97" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" t="s">
+        <v>296</v>
+      </c>
+      <c r="B98" t="s">
         <v>297</v>
       </c>
-      <c r="B98" t="s">
+      <c r="C98" t="s">
+        <v>6</v>
+      </c>
+      <c r="D98" t="s">
         <v>298</v>
-      </c>
-      <c r="C98" t="s">
-        <v>6</v>
-      </c>
-      <c r="D98" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" t="s">
+        <v>299</v>
+      </c>
+      <c r="B99" t="s">
         <v>300</v>
       </c>
-      <c r="B99" t="s">
+      <c r="C99" t="s">
+        <v>6</v>
+      </c>
+      <c r="D99" t="s">
         <v>301</v>
-      </c>
-      <c r="C99" t="s">
-        <v>6</v>
-      </c>
-      <c r="D99" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" t="s">
+        <v>302</v>
+      </c>
+      <c r="B100" t="s">
         <v>303</v>
       </c>
-      <c r="B100" t="s">
+      <c r="C100" t="s">
+        <v>6</v>
+      </c>
+      <c r="D100" t="s">
         <v>304</v>
-      </c>
-      <c r="C100" t="s">
-        <v>6</v>
-      </c>
-      <c r="D100" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="101" spans="1:4">
       <c r="A101" t="s">
+        <v>305</v>
+      </c>
+      <c r="B101" t="s">
         <v>306</v>
       </c>
-      <c r="B101" t="s">
+      <c r="C101" t="s">
+        <v>6</v>
+      </c>
+      <c r="D101" t="s">
         <v>307</v>
-      </c>
-      <c r="C101" t="s">
-        <v>6</v>
-      </c>
-      <c r="D101" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" t="s">
+        <v>308</v>
+      </c>
+      <c r="B102" t="s">
         <v>309</v>
       </c>
-      <c r="B102" t="s">
+      <c r="C102" t="s">
+        <v>6</v>
+      </c>
+      <c r="D102" t="s">
         <v>310</v>
-      </c>
-      <c r="C102" t="s">
-        <v>6</v>
-      </c>
-      <c r="D102" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" t="s">
+        <v>311</v>
+      </c>
+      <c r="B103" t="s">
         <v>312</v>
       </c>
-      <c r="B103" t="s">
+      <c r="C103" t="s">
+        <v>6</v>
+      </c>
+      <c r="D103" t="s">
         <v>313</v>
-      </c>
-      <c r="C103" t="s">
-        <v>6</v>
-      </c>
-      <c r="D103" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="104" spans="1:4">
       <c r="A104" t="s">
+        <v>314</v>
+      </c>
+      <c r="B104" t="s">
         <v>315</v>
       </c>
-      <c r="B104" t="s">
+      <c r="C104" t="s">
+        <v>6</v>
+      </c>
+      <c r="D104" t="s">
         <v>316</v>
-      </c>
-      <c r="C104" t="s">
-        <v>6</v>
-      </c>
-      <c r="D104" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="105" spans="1:4">
       <c r="A105" t="s">
+        <v>317</v>
+      </c>
+      <c r="B105" t="s">
         <v>318</v>
       </c>
-      <c r="B105" t="s">
+      <c r="C105" t="s">
+        <v>6</v>
+      </c>
+      <c r="D105" t="s">
         <v>319</v>
-      </c>
-      <c r="C105" t="s">
-        <v>6</v>
-      </c>
-      <c r="D105" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="106" spans="1:4">
       <c r="A106" t="s">
+        <v>320</v>
+      </c>
+      <c r="B106" t="s">
         <v>321</v>
       </c>
-      <c r="B106" t="s">
+      <c r="C106" t="s">
+        <v>6</v>
+      </c>
+      <c r="D106" t="s">
         <v>322</v>
-      </c>
-      <c r="C106" t="s">
-        <v>6</v>
-      </c>
-      <c r="D106" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="107" spans="1:4">
       <c r="A107" t="s">
+        <v>323</v>
+      </c>
+      <c r="B107" t="s">
         <v>324</v>
       </c>
-      <c r="B107" t="s">
+      <c r="C107" t="s">
+        <v>6</v>
+      </c>
+      <c r="D107" t="s">
         <v>325</v>
-      </c>
-      <c r="C107" t="s">
-        <v>6</v>
-      </c>
-      <c r="D107" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="108" spans="1:4">
       <c r="A108" t="s">
+        <v>326</v>
+      </c>
+      <c r="B108" t="s">
         <v>327</v>
-      </c>
-      <c r="B108" t="s">
-        <v>328</v>
       </c>
       <c r="C108" t="s">
         <v>75</v>
       </c>
       <c r="D108" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="109" spans="1:4">
       <c r="A109" t="s">
+        <v>329</v>
+      </c>
+      <c r="B109" t="s">
         <v>330</v>
       </c>
-      <c r="B109" t="s">
+      <c r="C109" t="s">
+        <v>6</v>
+      </c>
+      <c r="D109" t="s">
         <v>331</v>
-      </c>
-      <c r="C109" t="s">
-        <v>6</v>
-      </c>
-      <c r="D109" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="110" spans="1:4">
       <c r="A110" t="s">
+        <v>332</v>
+      </c>
+      <c r="B110" t="s">
         <v>333</v>
-      </c>
-      <c r="B110" t="s">
-        <v>334</v>
       </c>
       <c r="C110" t="s">
         <v>75</v>
       </c>
       <c r="D110" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="111" spans="1:4">
       <c r="A111" t="s">
+        <v>335</v>
+      </c>
+      <c r="B111" t="s">
         <v>336</v>
       </c>
-      <c r="B111" t="s">
+      <c r="C111" t="s">
+        <v>6</v>
+      </c>
+      <c r="D111" t="s">
         <v>337</v>
-      </c>
-      <c r="C111" t="s">
-        <v>6</v>
-      </c>
-      <c r="D111" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="112" spans="1:4">
       <c r="A112" t="s">
+        <v>338</v>
+      </c>
+      <c r="B112" t="s">
         <v>339</v>
-      </c>
-      <c r="B112" t="s">
-        <v>340</v>
       </c>
       <c r="C112" t="s">
         <v>71</v>
       </c>
       <c r="D112" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" t="s">
+        <v>341</v>
+      </c>
+      <c r="B113" t="s">
         <v>342</v>
       </c>
-      <c r="B113" t="s">
+      <c r="C113" t="s">
+        <v>6</v>
+      </c>
+      <c r="D113" t="s">
         <v>343</v>
-      </c>
-      <c r="C113" t="s">
-        <v>6</v>
-      </c>
-      <c r="D113" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="114" spans="1:4">
       <c r="A114" t="s">
+        <v>344</v>
+      </c>
+      <c r="B114" t="s">
         <v>345</v>
       </c>
-      <c r="B114" t="s">
+      <c r="C114" t="s">
+        <v>6</v>
+      </c>
+      <c r="D114" t="s">
         <v>346</v>
-      </c>
-      <c r="C114" t="s">
-        <v>6</v>
-      </c>
-      <c r="D114" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="115" spans="1:4">
       <c r="A115" t="s">
+        <v>347</v>
+      </c>
+      <c r="B115" t="s">
         <v>348</v>
       </c>
-      <c r="B115" t="s">
+      <c r="C115" t="s">
+        <v>6</v>
+      </c>
+      <c r="D115" t="s">
         <v>349</v>
-      </c>
-      <c r="C115" t="s">
-        <v>6</v>
-      </c>
-      <c r="D115" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="116" spans="1:4">
       <c r="A116" t="s">
+        <v>350</v>
+      </c>
+      <c r="B116" t="s">
         <v>351</v>
-      </c>
-      <c r="B116" t="s">
-        <v>352</v>
       </c>
       <c r="C116" t="s">
         <v>79</v>
       </c>
       <c r="D116" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" t="s">
+        <v>353</v>
+      </c>
+      <c r="B117" t="s">
         <v>354</v>
       </c>
-      <c r="B117" t="s">
+      <c r="C117" t="s">
+        <v>6</v>
+      </c>
+      <c r="D117" t="s">
         <v>355</v>
-      </c>
-      <c r="C117" t="s">
-        <v>6</v>
-      </c>
-      <c r="D117" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" t="s">
+        <v>356</v>
+      </c>
+      <c r="B118" t="s">
         <v>357</v>
       </c>
-      <c r="B118" t="s">
+      <c r="C118" t="s">
+        <v>6</v>
+      </c>
+      <c r="D118" t="s">
         <v>358</v>
-      </c>
-      <c r="C118" t="s">
-        <v>6</v>
-      </c>
-      <c r="D118" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="119" spans="1:4">
       <c r="A119" t="s">
+        <v>359</v>
+      </c>
+      <c r="B119" t="s">
         <v>360</v>
-      </c>
-      <c r="B119" t="s">
-        <v>361</v>
       </c>
       <c r="C119" t="s">
         <v>179</v>
       </c>
       <c r="D119" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="120" spans="1:4">
       <c r="A120" t="s">
+        <v>362</v>
+      </c>
+      <c r="B120" t="s">
         <v>363</v>
       </c>
-      <c r="B120" t="s">
+      <c r="C120" t="s">
+        <v>6</v>
+      </c>
+      <c r="D120" t="s">
         <v>364</v>
-      </c>
-      <c r="C120" t="s">
-        <v>6</v>
-      </c>
-      <c r="D120" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="121" spans="1:4">
       <c r="A121" t="s">
+        <v>365</v>
+      </c>
+      <c r="B121" t="s">
         <v>366</v>
-      </c>
-      <c r="B121" t="s">
-        <v>367</v>
       </c>
       <c r="C121" t="s">
         <v>79</v>
       </c>
       <c r="D121" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="122" spans="1:4">
       <c r="A122" t="s">
+        <v>368</v>
+      </c>
+      <c r="B122" t="s">
         <v>369</v>
       </c>
-      <c r="B122" t="s">
+      <c r="C122" t="s">
+        <v>6</v>
+      </c>
+      <c r="D122" t="s">
         <v>370</v>
-      </c>
-      <c r="C122" t="s">
-        <v>6</v>
-      </c>
-      <c r="D122" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="123" spans="1:4">
       <c r="A123" t="s">
+        <v>371</v>
+      </c>
+      <c r="B123" t="s">
         <v>372</v>
       </c>
-      <c r="B123" t="s">
+      <c r="C123" t="s">
+        <v>6</v>
+      </c>
+      <c r="D123" t="s">
         <v>373</v>
-      </c>
-      <c r="C123" t="s">
-        <v>6</v>
-      </c>
-      <c r="D123" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="124" spans="1:4">
       <c r="A124" t="s">
+        <v>374</v>
+      </c>
+      <c r="B124" t="s">
         <v>375</v>
-      </c>
-      <c r="B124" t="s">
-        <v>376</v>
       </c>
       <c r="C124" t="s">
         <v>75</v>
       </c>
       <c r="D124" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="125" spans="1:4">
       <c r="A125" t="s">
+        <v>377</v>
+      </c>
+      <c r="B125" t="s">
         <v>378</v>
       </c>
-      <c r="B125" t="s">
+      <c r="C125" t="s">
+        <v>6</v>
+      </c>
+      <c r="D125" t="s">
         <v>379</v>
-      </c>
-      <c r="C125" t="s">
-        <v>6</v>
-      </c>
-      <c r="D125" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" t="s">
+        <v>380</v>
+      </c>
+      <c r="B126" t="s">
         <v>381</v>
-      </c>
-      <c r="B126" t="s">
-        <v>382</v>
       </c>
       <c r="C126" t="s">
         <v>55</v>
       </c>
       <c r="D126" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="127" spans="1:4">
       <c r="A127" t="s">
+        <v>383</v>
+      </c>
+      <c r="B127" t="s">
         <v>384</v>
       </c>
-      <c r="B127" t="s">
+      <c r="C127" t="s">
+        <v>6</v>
+      </c>
+      <c r="D127" t="s">
         <v>385</v>
-      </c>
-      <c r="C127" t="s">
-        <v>6</v>
-      </c>
-      <c r="D127" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" t="s">
+        <v>386</v>
+      </c>
+      <c r="B128" t="s">
         <v>387</v>
       </c>
-      <c r="B128" t="s">
+      <c r="C128" t="s">
+        <v>6</v>
+      </c>
+      <c r="D128" t="s">
         <v>388</v>
-      </c>
-      <c r="C128" t="s">
-        <v>6</v>
-      </c>
-      <c r="D128" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="129" spans="1:4">
       <c r="A129" t="s">
+        <v>389</v>
+      </c>
+      <c r="B129" t="s">
         <v>390</v>
-      </c>
-      <c r="B129" t="s">
-        <v>391</v>
       </c>
       <c r="C129" t="s">
         <v>75</v>
       </c>
       <c r="D129" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="130" spans="1:4">
       <c r="A130" t="s">
+        <v>392</v>
+      </c>
+      <c r="B130" t="s">
         <v>393</v>
       </c>
-      <c r="B130" t="s">
+      <c r="C130" t="s">
+        <v>6</v>
+      </c>
+      <c r="D130" t="s">
         <v>394</v>
-      </c>
-      <c r="C130" t="s">
-        <v>6</v>
-      </c>
-      <c r="D130" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="131" spans="1:4">
       <c r="A131" t="s">
+        <v>395</v>
+      </c>
+      <c r="B131" t="s">
         <v>396</v>
-      </c>
-      <c r="B131" t="s">
-        <v>397</v>
       </c>
       <c r="C131" t="s">
         <v>71</v>
       </c>
       <c r="D131" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="132" spans="1:4">
       <c r="A132" t="s">
+        <v>398</v>
+      </c>
+      <c r="B132" t="s">
         <v>399</v>
-      </c>
-      <c r="B132" t="s">
-        <v>400</v>
       </c>
       <c r="C132" t="s">
         <v>75</v>
       </c>
       <c r="D132" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="133" spans="1:4">
       <c r="A133" t="s">
+        <v>401</v>
+      </c>
+      <c r="B133" t="s">
+        <v>401</v>
+      </c>
+      <c r="C133" t="s">
+        <v>6</v>
+      </c>
+      <c r="D133" t="s">
         <v>402</v>
-      </c>
-      <c r="B133" t="s">
-        <v>402</v>
-      </c>
-      <c r="C133" t="s">
-        <v>6</v>
-      </c>
-      <c r="D133" t="s">
-        <v>403</v>
       </c>
     </row>
     <row r="134" spans="1:4">
       <c r="A134" t="s">
+        <v>403</v>
+      </c>
+      <c r="B134" t="s">
         <v>404</v>
       </c>
-      <c r="B134" t="s">
+      <c r="C134" t="s">
+        <v>6</v>
+      </c>
+      <c r="D134" t="s">
         <v>405</v>
-      </c>
-      <c r="C134" t="s">
-        <v>6</v>
-      </c>
-      <c r="D134" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="135" spans="1:4">
       <c r="A135" t="s">
+        <v>406</v>
+      </c>
+      <c r="B135" t="s">
         <v>407</v>
-      </c>
-      <c r="B135" t="s">
-        <v>408</v>
       </c>
       <c r="C135" t="s">
         <v>71</v>
       </c>
       <c r="D135" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="136" spans="1:4">
       <c r="A136" t="s">
+        <v>409</v>
+      </c>
+      <c r="B136" t="s">
         <v>410</v>
       </c>
-      <c r="B136" t="s">
+      <c r="C136" t="s">
+        <v>6</v>
+      </c>
+      <c r="D136" t="s">
         <v>411</v>
-      </c>
-      <c r="C136" t="s">
-        <v>6</v>
-      </c>
-      <c r="D136" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="137" spans="1:4">
       <c r="A137" t="s">
+        <v>412</v>
+      </c>
+      <c r="B137" t="s">
         <v>413</v>
-      </c>
-      <c r="B137" t="s">
-        <v>414</v>
       </c>
       <c r="C137" t="s">
         <v>79</v>
       </c>
       <c r="D137" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="138" spans="1:4">
       <c r="A138" t="s">
+        <v>415</v>
+      </c>
+      <c r="B138" t="s">
         <v>416</v>
       </c>
-      <c r="B138" t="s">
+      <c r="C138" t="s">
+        <v>6</v>
+      </c>
+      <c r="D138" t="s">
         <v>417</v>
-      </c>
-      <c r="C138" t="s">
-        <v>6</v>
-      </c>
-      <c r="D138" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="139" spans="1:4">
       <c r="A139" t="s">
+        <v>418</v>
+      </c>
+      <c r="B139" t="s">
         <v>419</v>
-      </c>
-      <c r="B139" t="s">
-        <v>420</v>
       </c>
       <c r="C139" t="s">
         <v>179</v>
       </c>
       <c r="D139" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="140" spans="1:4">
       <c r="A140" t="s">
+        <v>421</v>
+      </c>
+      <c r="B140" t="s">
         <v>422</v>
       </c>
-      <c r="B140" t="s">
+      <c r="C140" t="s">
+        <v>6</v>
+      </c>
+      <c r="D140" t="s">
         <v>423</v>
-      </c>
-      <c r="C140" t="s">
-        <v>6</v>
-      </c>
-      <c r="D140" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="141" spans="1:4">
       <c r="A141" t="s">
+        <v>424</v>
+      </c>
+      <c r="B141" t="s">
         <v>425</v>
-      </c>
-      <c r="B141" t="s">
-        <v>426</v>
       </c>
       <c r="C141" t="s">
         <v>75</v>
       </c>
       <c r="D141" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="142" spans="1:4">
       <c r="A142" t="s">
+        <v>427</v>
+      </c>
+      <c r="B142" t="s">
         <v>428</v>
       </c>
-      <c r="B142" t="s">
+      <c r="C142" t="s">
+        <v>6</v>
+      </c>
+      <c r="D142" t="s">
         <v>429</v>
-      </c>
-      <c r="C142" t="s">
-        <v>6</v>
-      </c>
-      <c r="D142" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="143" spans="1:4">
       <c r="A143" t="s">
+        <v>430</v>
+      </c>
+      <c r="B143" t="s">
+        <v>430</v>
+      </c>
+      <c r="C143" t="s">
+        <v>6</v>
+      </c>
+      <c r="D143" t="s">
         <v>431</v>
-      </c>
-      <c r="B143" t="s">
-        <v>431</v>
-      </c>
-      <c r="C143" t="s">
-        <v>6</v>
-      </c>
-      <c r="D143" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="144" spans="1:4">
       <c r="A144" t="s">
+        <v>432</v>
+      </c>
+      <c r="B144" t="s">
         <v>433</v>
       </c>
-      <c r="B144" t="s">
+      <c r="C144" t="s">
+        <v>6</v>
+      </c>
+      <c r="D144" t="s">
         <v>434</v>
-      </c>
-      <c r="C144" t="s">
-        <v>6</v>
-      </c>
-      <c r="D144" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="145" spans="1:4">
       <c r="A145" t="s">
+        <v>435</v>
+      </c>
+      <c r="B145" t="s">
         <v>436</v>
-      </c>
-      <c r="B145" t="s">
-        <v>437</v>
       </c>
       <c r="C145" t="s">
         <v>79</v>
       </c>
       <c r="D145" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="146" spans="1:4">
       <c r="A146" t="s">
+        <v>438</v>
+      </c>
+      <c r="B146" t="s">
         <v>439</v>
       </c>
-      <c r="B146" t="s">
+      <c r="C146" t="s">
+        <v>6</v>
+      </c>
+      <c r="D146" t="s">
         <v>440</v>
-      </c>
-      <c r="C146" t="s">
-        <v>6</v>
-      </c>
-      <c r="D146" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="147" spans="1:4">
       <c r="A147" t="s">
+        <v>441</v>
+      </c>
+      <c r="B147" t="s">
         <v>442</v>
-      </c>
-      <c r="B147" t="s">
-        <v>443</v>
       </c>
       <c r="C147" t="s">
         <v>71</v>
       </c>
       <c r="D147" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="148" spans="1:4">
       <c r="A148" t="s">
+        <v>444</v>
+      </c>
+      <c r="B148" t="s">
         <v>445</v>
       </c>
-      <c r="B148" t="s">
+      <c r="C148" t="s">
+        <v>6</v>
+      </c>
+      <c r="D148" t="s">
         <v>446</v>
-      </c>
-      <c r="C148" t="s">
-        <v>6</v>
-      </c>
-      <c r="D148" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="149" spans="1:4">
       <c r="A149" t="s">
+        <v>447</v>
+      </c>
+      <c r="B149" t="s">
         <v>448</v>
       </c>
-      <c r="B149" t="s">
+      <c r="C149" t="s">
+        <v>6</v>
+      </c>
+      <c r="D149" t="s">
         <v>449</v>
-      </c>
-      <c r="C149" t="s">
-        <v>6</v>
-      </c>
-      <c r="D149" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="150" spans="1:4">
       <c r="A150" t="s">
+        <v>450</v>
+      </c>
+      <c r="B150" t="s">
         <v>451</v>
       </c>
-      <c r="B150" t="s">
+      <c r="C150" t="s">
+        <v>6</v>
+      </c>
+      <c r="D150" t="s">
         <v>452</v>
-      </c>
-      <c r="C150" t="s">
-        <v>6</v>
-      </c>
-      <c r="D150" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="151" spans="1:4">
       <c r="A151" t="s">
+        <v>453</v>
+      </c>
+      <c r="B151" t="s">
         <v>454</v>
       </c>
-      <c r="B151" t="s">
+      <c r="C151" t="s">
+        <v>6</v>
+      </c>
+      <c r="D151" t="s">
         <v>455</v>
-      </c>
-      <c r="C151" t="s">
-        <v>6</v>
-      </c>
-      <c r="D151" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="152" spans="1:4">
       <c r="A152" t="s">
+        <v>456</v>
+      </c>
+      <c r="B152" t="s">
         <v>457</v>
       </c>
-      <c r="B152" t="s">
+      <c r="C152" t="s">
+        <v>6</v>
+      </c>
+      <c r="D152" t="s">
         <v>458</v>
-      </c>
-      <c r="C152" t="s">
-        <v>6</v>
-      </c>
-      <c r="D152" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="153" spans="1:4">
       <c r="A153" t="s">
+        <v>459</v>
+      </c>
+      <c r="B153" t="s">
+        <v>459</v>
+      </c>
+      <c r="C153" t="s">
         <v>460</v>
       </c>
-      <c r="B153" t="s">
-        <v>460</v>
-      </c>
-      <c r="C153" t="s">
+      <c r="D153" t="s">
         <v>461</v>
-      </c>
-      <c r="D153" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="154" spans="1:4">
       <c r="A154" t="s">
+        <v>462</v>
+      </c>
+      <c r="B154" t="s">
         <v>463</v>
-      </c>
-      <c r="B154" t="s">
-        <v>464</v>
       </c>
       <c r="C154" t="s">
         <v>79</v>
       </c>
       <c r="D154" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="155" spans="1:4">
       <c r="A155" t="s">
+        <v>465</v>
+      </c>
+      <c r="B155" t="s">
         <v>466</v>
       </c>
-      <c r="B155" t="s">
+      <c r="C155" t="s">
+        <v>6</v>
+      </c>
+      <c r="D155" t="s">
         <v>467</v>
-      </c>
-      <c r="C155" t="s">
-        <v>6</v>
-      </c>
-      <c r="D155" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="156" spans="1:4">
       <c r="A156" t="s">
+        <v>468</v>
+      </c>
+      <c r="B156" t="s">
         <v>469</v>
-      </c>
-      <c r="B156" t="s">
-        <v>470</v>
       </c>
       <c r="C156" t="s">
         <v>75</v>
       </c>
       <c r="D156" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="157" spans="1:4">
       <c r="A157" t="s">
+        <v>471</v>
+      </c>
+      <c r="B157" t="s">
         <v>472</v>
-      </c>
-      <c r="B157" t="s">
-        <v>473</v>
       </c>
       <c r="C157" t="s">
         <v>75</v>
       </c>
       <c r="D157" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="158" spans="1:4">
       <c r="A158" t="s">
+        <v>474</v>
+      </c>
+      <c r="B158" t="s">
         <v>475</v>
       </c>
-      <c r="B158" t="s">
+      <c r="C158" t="s">
+        <v>6</v>
+      </c>
+      <c r="D158" t="s">
         <v>476</v>
-      </c>
-      <c r="C158" t="s">
-        <v>6</v>
-      </c>
-      <c r="D158" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="159" spans="1:4">
       <c r="A159" t="s">
+        <v>477</v>
+      </c>
+      <c r="B159" t="s">
         <v>478</v>
-      </c>
-      <c r="B159" t="s">
-        <v>479</v>
       </c>
       <c r="C159" t="s">
         <v>55</v>
       </c>
       <c r="D159" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="160" spans="1:4">
       <c r="A160" t="s">
+        <v>480</v>
+      </c>
+      <c r="B160" t="s">
         <v>481</v>
       </c>
-      <c r="B160" t="s">
+      <c r="C160" t="s">
+        <v>6</v>
+      </c>
+      <c r="D160" t="s">
         <v>482</v>
-      </c>
-      <c r="C160" t="s">
-        <v>6</v>
-      </c>
-      <c r="D160" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="161" spans="1:4">
       <c r="A161" t="s">
+        <v>483</v>
+      </c>
+      <c r="B161" t="s">
         <v>484</v>
       </c>
-      <c r="B161" t="s">
+      <c r="C161" t="s">
+        <v>6</v>
+      </c>
+      <c r="D161" t="s">
         <v>485</v>
-      </c>
-      <c r="C161" t="s">
-        <v>6</v>
-      </c>
-      <c r="D161" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="162" spans="1:4">
       <c r="A162" t="s">
+        <v>486</v>
+      </c>
+      <c r="B162" t="s">
         <v>487</v>
       </c>
-      <c r="B162" t="s">
+      <c r="C162" t="s">
+        <v>6</v>
+      </c>
+      <c r="D162" t="s">
         <v>488</v>
-      </c>
-      <c r="C162" t="s">
-        <v>6</v>
-      </c>
-      <c r="D162" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="163" spans="1:4">
       <c r="A163" t="s">
+        <v>489</v>
+      </c>
+      <c r="B163" t="s">
+        <v>489</v>
+      </c>
+      <c r="C163" t="s">
+        <v>6</v>
+      </c>
+      <c r="D163" t="s">
         <v>490</v>
-      </c>
-      <c r="B163" t="s">
-        <v>490</v>
-      </c>
-      <c r="C163" t="s">
-        <v>6</v>
-      </c>
-      <c r="D163" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="164" spans="1:4">
       <c r="A164" t="s">
+        <v>491</v>
+      </c>
+      <c r="B164" t="s">
         <v>492</v>
       </c>
-      <c r="B164" t="s">
+      <c r="C164" t="s">
+        <v>6</v>
+      </c>
+      <c r="D164" t="s">
         <v>493</v>
-      </c>
-      <c r="C164" t="s">
-        <v>6</v>
-      </c>
-      <c r="D164" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="165" spans="1:4">
       <c r="A165" t="s">
+        <v>494</v>
+      </c>
+      <c r="B165" t="s">
         <v>495</v>
       </c>
-      <c r="B165" t="s">
+      <c r="C165" t="s">
+        <v>6</v>
+      </c>
+      <c r="D165" t="s">
         <v>496</v>
-      </c>
-      <c r="C165" t="s">
-        <v>6</v>
-      </c>
-      <c r="D165" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="166" spans="1:4">
       <c r="A166" t="s">
+        <v>497</v>
+      </c>
+      <c r="B166" t="s">
         <v>498</v>
-      </c>
-      <c r="B166" t="s">
-        <v>499</v>
       </c>
       <c r="C166" t="s">
         <v>75</v>
       </c>
       <c r="D166" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="167" spans="1:4">
       <c r="A167" t="s">
+        <v>500</v>
+      </c>
+      <c r="B167" t="s">
         <v>501</v>
-      </c>
-      <c r="B167" t="s">
-        <v>502</v>
       </c>
       <c r="C167" t="s">
         <v>79</v>
       </c>
       <c r="D167" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="168" spans="1:4">
       <c r="A168" t="s">
+        <v>503</v>
+      </c>
+      <c r="B168" t="s">
         <v>504</v>
       </c>
-      <c r="B168" t="s">
+      <c r="C168" t="s">
+        <v>6</v>
+      </c>
+      <c r="D168" t="s">
         <v>505</v>
-      </c>
-      <c r="C168" t="s">
-        <v>6</v>
-      </c>
-      <c r="D168" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="169" spans="1:4">
       <c r="A169" t="s">
+        <v>506</v>
+      </c>
+      <c r="B169" t="s">
         <v>507</v>
       </c>
-      <c r="B169" t="s">
+      <c r="C169" t="s">
+        <v>6</v>
+      </c>
+      <c r="D169" t="s">
         <v>508</v>
-      </c>
-      <c r="C169" t="s">
-        <v>6</v>
-      </c>
-      <c r="D169" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="170" spans="1:4">
       <c r="A170" t="s">
+        <v>509</v>
+      </c>
+      <c r="B170" t="s">
         <v>510</v>
       </c>
-      <c r="B170" t="s">
+      <c r="C170" t="s">
+        <v>6</v>
+      </c>
+      <c r="D170" t="s">
         <v>511</v>
-      </c>
-      <c r="C170" t="s">
-        <v>6</v>
-      </c>
-      <c r="D170" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="171" spans="1:4">
       <c r="A171" t="s">
+        <v>512</v>
+      </c>
+      <c r="B171" t="s">
         <v>513</v>
       </c>
-      <c r="B171" t="s">
+      <c r="C171" t="s">
+        <v>6</v>
+      </c>
+      <c r="D171" t="s">
         <v>514</v>
-      </c>
-      <c r="C171" t="s">
-        <v>6</v>
-      </c>
-      <c r="D171" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="172" spans="1:4">
       <c r="A172" t="s">
+        <v>515</v>
+      </c>
+      <c r="B172" t="s">
         <v>516</v>
       </c>
-      <c r="B172" t="s">
+      <c r="C172" t="s">
+        <v>6</v>
+      </c>
+      <c r="D172" t="s">
         <v>517</v>
-      </c>
-      <c r="C172" t="s">
-        <v>6</v>
-      </c>
-      <c r="D172" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="173" spans="1:4">
       <c r="A173" t="s">
+        <v>518</v>
+      </c>
+      <c r="B173" t="s">
         <v>519</v>
-      </c>
-      <c r="B173" t="s">
-        <v>520</v>
       </c>
       <c r="C173" t="s">
         <v>71</v>
       </c>
       <c r="D173" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="174" spans="1:4">
       <c r="A174" t="s">
+        <v>521</v>
+      </c>
+      <c r="B174" t="s">
         <v>522</v>
-      </c>
-      <c r="B174" t="s">
-        <v>523</v>
       </c>
       <c r="C174" t="s">
         <v>179</v>
       </c>
       <c r="D174" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="175" spans="1:4">
       <c r="A175" t="s">
+        <v>524</v>
+      </c>
+      <c r="B175" t="s">
         <v>525</v>
       </c>
-      <c r="B175" t="s">
+      <c r="C175" t="s">
+        <v>6</v>
+      </c>
+      <c r="D175" t="s">
         <v>526</v>
-      </c>
-      <c r="C175" t="s">
-        <v>6</v>
-      </c>
-      <c r="D175" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="176" spans="1:4">
       <c r="A176" t="s">
+        <v>527</v>
+      </c>
+      <c r="B176" t="s">
         <v>528</v>
       </c>
-      <c r="B176" t="s">
+      <c r="C176" t="s">
+        <v>6</v>
+      </c>
+      <c r="D176" t="s">
         <v>529</v>
-      </c>
-      <c r="C176" t="s">
-        <v>6</v>
-      </c>
-      <c r="D176" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="177" spans="1:4">
       <c r="A177" t="s">
+        <v>530</v>
+      </c>
+      <c r="B177" t="s">
         <v>531</v>
-      </c>
-      <c r="B177" t="s">
-        <v>532</v>
       </c>
       <c r="C177" t="s">
         <v>55</v>
       </c>
       <c r="D177" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="178" spans="1:4">
       <c r="A178" t="s">
+        <v>533</v>
+      </c>
+      <c r="B178" t="s">
         <v>534</v>
-      </c>
-      <c r="B178" t="s">
-        <v>535</v>
       </c>
       <c r="C178" t="s">
         <v>55</v>
       </c>
       <c r="D178" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="179" spans="1:4">
       <c r="A179" t="s">
+        <v>536</v>
+      </c>
+      <c r="B179" t="s">
         <v>537</v>
-      </c>
-      <c r="B179" t="s">
-        <v>538</v>
       </c>
       <c r="C179" t="s">
         <v>79</v>
       </c>
       <c r="D179" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="180" spans="1:4">
       <c r="A180" t="s">
+        <v>539</v>
+      </c>
+      <c r="B180" t="s">
         <v>540</v>
       </c>
-      <c r="B180" t="s">
+      <c r="C180" t="s">
+        <v>6</v>
+      </c>
+      <c r="D180" t="s">
         <v>541</v>
-      </c>
-      <c r="C180" t="s">
-        <v>6</v>
-      </c>
-      <c r="D180" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="181" spans="1:4">
       <c r="A181" t="s">
+        <v>542</v>
+      </c>
+      <c r="B181" t="s">
         <v>543</v>
       </c>
-      <c r="B181" t="s">
+      <c r="C181" t="s">
+        <v>6</v>
+      </c>
+      <c r="D181" t="s">
         <v>544</v>
-      </c>
-      <c r="C181" t="s">
-        <v>6</v>
-      </c>
-      <c r="D181" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="182" spans="1:4">
       <c r="A182" t="s">
+        <v>545</v>
+      </c>
+      <c r="B182" t="s">
         <v>546</v>
       </c>
-      <c r="B182" t="s">
+      <c r="C182" t="s">
+        <v>6</v>
+      </c>
+      <c r="D182" t="s">
         <v>547</v>
-      </c>
-      <c r="C182" t="s">
-        <v>6</v>
-      </c>
-      <c r="D182" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="183" spans="1:4">
       <c r="A183" t="s">
+        <v>548</v>
+      </c>
+      <c r="B183" t="s">
         <v>549</v>
       </c>
-      <c r="B183" t="s">
+      <c r="C183" t="s">
+        <v>6</v>
+      </c>
+      <c r="D183" t="s">
         <v>550</v>
-      </c>
-      <c r="C183" t="s">
-        <v>6</v>
-      </c>
-      <c r="D183" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="184" spans="1:4">
       <c r="A184" t="s">
+        <v>551</v>
+      </c>
+      <c r="B184" t="s">
         <v>552</v>
-      </c>
-      <c r="B184" t="s">
-        <v>553</v>
       </c>
       <c r="C184" t="s">
         <v>179</v>
       </c>
       <c r="D184" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="185" spans="1:4">
       <c r="A185" t="s">
+        <v>554</v>
+      </c>
+      <c r="B185" t="s">
         <v>555</v>
-      </c>
-      <c r="B185" t="s">
-        <v>556</v>
       </c>
       <c r="C185" t="s">
         <v>79</v>
       </c>
       <c r="D185" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="186" spans="1:4">
       <c r="A186" t="s">
+        <v>557</v>
+      </c>
+      <c r="B186" t="s">
         <v>558</v>
-      </c>
-      <c r="B186" t="s">
-        <v>559</v>
       </c>
       <c r="C186" t="s">
         <v>79</v>
       </c>
       <c r="D186" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="187" spans="1:4">
       <c r="A187" t="s">
+        <v>560</v>
+      </c>
+      <c r="B187" t="s">
         <v>561</v>
       </c>
-      <c r="B187" t="s">
+      <c r="C187" t="s">
+        <v>6</v>
+      </c>
+      <c r="D187" t="s">
         <v>562</v>
-      </c>
-      <c r="C187" t="s">
-        <v>6</v>
-      </c>
-      <c r="D187" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="188" spans="1:4">
       <c r="A188" t="s">
+        <v>563</v>
+      </c>
+      <c r="B188" t="s">
         <v>564</v>
       </c>
-      <c r="B188" t="s">
+      <c r="C188" t="s">
+        <v>6</v>
+      </c>
+      <c r="D188" t="s">
         <v>565</v>
-      </c>
-      <c r="C188" t="s">
-        <v>6</v>
-      </c>
-      <c r="D188" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="189" spans="1:4">
       <c r="A189" t="s">
+        <v>566</v>
+      </c>
+      <c r="B189" t="s">
         <v>567</v>
       </c>
-      <c r="B189" t="s">
+      <c r="C189" t="s">
+        <v>6</v>
+      </c>
+      <c r="D189" t="s">
         <v>568</v>
-      </c>
-      <c r="C189" t="s">
-        <v>6</v>
-      </c>
-      <c r="D189" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="190" spans="1:4">
       <c r="A190" t="s">
+        <v>569</v>
+      </c>
+      <c r="B190" t="s">
         <v>570</v>
-      </c>
-      <c r="B190" t="s">
-        <v>571</v>
       </c>
       <c r="C190" t="s">
         <v>79</v>
       </c>
       <c r="D190" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="191" spans="1:4">
       <c r="A191" t="s">
+        <v>572</v>
+      </c>
+      <c r="B191" t="s">
         <v>573</v>
-      </c>
-      <c r="B191" t="s">
-        <v>574</v>
       </c>
       <c r="C191" t="s">
         <v>75</v>
       </c>
       <c r="D191" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="192" spans="1:4">
       <c r="A192" t="s">
+        <v>575</v>
+      </c>
+      <c r="B192" t="s">
         <v>576</v>
       </c>
-      <c r="B192" t="s">
+      <c r="C192" t="s">
+        <v>6</v>
+      </c>
+      <c r="D192" t="s">
         <v>577</v>
-      </c>
-      <c r="C192" t="s">
-        <v>6</v>
-      </c>
-      <c r="D192" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="193" spans="1:4">
       <c r="A193" t="s">
+        <v>578</v>
+      </c>
+      <c r="B193" t="s">
         <v>579</v>
-      </c>
-      <c r="B193" t="s">
-        <v>580</v>
       </c>
       <c r="C193" t="s">
         <v>55</v>
       </c>
       <c r="D193" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="194" spans="1:4">
       <c r="A194" t="s">
+        <v>581</v>
+      </c>
+      <c r="B194" t="s">
         <v>582</v>
-      </c>
-      <c r="B194" t="s">
-        <v>583</v>
       </c>
       <c r="C194" t="s">
         <v>55</v>
       </c>
       <c r="D194" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="195" spans="1:4">
       <c r="A195" t="s">
+        <v>584</v>
+      </c>
+      <c r="B195" t="s">
         <v>585</v>
       </c>
-      <c r="B195" t="s">
+      <c r="C195" t="s">
+        <v>6</v>
+      </c>
+      <c r="D195" t="s">
         <v>586</v>
-      </c>
-      <c r="C195" t="s">
-        <v>6</v>
-      </c>
-      <c r="D195" t="s">
-        <v>587</v>
       </c>
     </row>
     <row r="196" spans="1:4">
       <c r="A196" t="s">
+        <v>587</v>
+      </c>
+      <c r="B196" t="s">
         <v>588</v>
       </c>
-      <c r="B196" t="s">
+      <c r="C196" t="s">
+        <v>6</v>
+      </c>
+      <c r="D196" t="s">
         <v>589</v>
-      </c>
-      <c r="C196" t="s">
-        <v>6</v>
-      </c>
-      <c r="D196" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="197" spans="1:4">
       <c r="A197" t="s">
+        <v>590</v>
+      </c>
+      <c r="B197" t="s">
         <v>591</v>
-      </c>
-      <c r="B197" t="s">
-        <v>592</v>
       </c>
       <c r="C197" t="s">
         <v>79</v>
       </c>
       <c r="D197" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="198" spans="1:4">
       <c r="A198" t="s">
+        <v>593</v>
+      </c>
+      <c r="B198" t="s">
         <v>594</v>
       </c>
-      <c r="B198" t="s">
+      <c r="C198" t="s">
+        <v>6</v>
+      </c>
+      <c r="D198" t="s">
         <v>595</v>
-      </c>
-      <c r="C198" t="s">
-        <v>6</v>
-      </c>
-      <c r="D198" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="199" spans="1:4">
       <c r="A199" t="s">
+        <v>596</v>
+      </c>
+      <c r="B199" t="s">
         <v>597</v>
       </c>
-      <c r="B199" t="s">
+      <c r="C199" t="s">
+        <v>6</v>
+      </c>
+      <c r="D199" t="s">
         <v>598</v>
-      </c>
-      <c r="C199" t="s">
-        <v>6</v>
-      </c>
-      <c r="D199" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="200" spans="1:4">
       <c r="A200" t="s">
+        <v>599</v>
+      </c>
+      <c r="B200" t="s">
         <v>600</v>
       </c>
-      <c r="B200" t="s">
+      <c r="C200" t="s">
+        <v>6</v>
+      </c>
+      <c r="D200" t="s">
         <v>601</v>
-      </c>
-      <c r="C200" t="s">
-        <v>6</v>
-      </c>
-      <c r="D200" t="s">
-        <v>602</v>
       </c>
     </row>
     <row r="201" spans="1:4">
       <c r="A201" t="s">
+        <v>602</v>
+      </c>
+      <c r="B201" t="s">
         <v>603</v>
       </c>
-      <c r="B201" t="s">
+      <c r="C201" t="s">
+        <v>6</v>
+      </c>
+      <c r="D201" t="s">
         <v>604</v>
-      </c>
-      <c r="C201" t="s">
-        <v>6</v>
-      </c>
-      <c r="D201" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="202" spans="1:4">
       <c r="A202" t="s">
+        <v>605</v>
+      </c>
+      <c r="B202" t="s">
         <v>606</v>
-      </c>
-      <c r="B202" t="s">
-        <v>607</v>
       </c>
       <c r="C202" t="s">
         <v>55</v>
       </c>
       <c r="D202" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="203" spans="1:4">
       <c r="A203" t="s">
+        <v>608</v>
+      </c>
+      <c r="B203" t="s">
         <v>609</v>
-      </c>
-      <c r="B203" t="s">
-        <v>610</v>
       </c>
       <c r="C203" t="s">
         <v>55</v>
       </c>
       <c r="D203" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="204" spans="1:4">
       <c r="A204" t="s">
+        <v>611</v>
+      </c>
+      <c r="B204" t="s">
         <v>612</v>
-      </c>
-      <c r="B204" t="s">
-        <v>613</v>
       </c>
       <c r="C204" t="s">
         <v>79</v>
       </c>
       <c r="D204" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="205" spans="1:4">
       <c r="A205" t="s">
+        <v>614</v>
+      </c>
+      <c r="B205" t="s">
         <v>615</v>
-      </c>
-      <c r="B205" t="s">
-        <v>616</v>
       </c>
       <c r="C205" t="s">
         <v>75</v>
       </c>
       <c r="D205" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="206" spans="1:4">
       <c r="A206" t="s">
+        <v>617</v>
+      </c>
+      <c r="B206" t="s">
         <v>618</v>
       </c>
-      <c r="B206" t="s">
+      <c r="C206" t="s">
+        <v>6</v>
+      </c>
+      <c r="D206" t="s">
         <v>619</v>
-      </c>
-      <c r="C206" t="s">
-        <v>6</v>
-      </c>
-      <c r="D206" t="s">
-        <v>620</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Skill information translation. (~140)
</commit_message>
<xml_diff>
--- a/skill.xlsx
+++ b/skill.xlsx
@@ -973,325 +973,325 @@
     <t>업물(業物) + 반동경감+2(反動軽減+2) + 정령의 가호(精霊の加護) + 체술+1(体術+1)</t>
   </si>
   <si>
-    <t>燼滅刃</t>
-  </si>
-  <si>
-    <t>燼滅刃の魂</t>
-  </si>
-  <si>
-    <t>斬れ味レベル+2 + 弾導強化 + 砥石使用高速化</t>
-  </si>
-  <si>
-    <t>真・鎧裂</t>
-  </si>
-  <si>
-    <t>真・鎧裂の魂</t>
-  </si>
-  <si>
-    <t>ガード性能+2 + 納刀術 + 刃鱗磨き</t>
-  </si>
-  <si>
-    <t>刃鱗</t>
-  </si>
-  <si>
-    <t>刃鱗磨き</t>
-  </si>
-  <si>
-    <t>抜刀中に回避行動により効果発動。剣士は斬れ味5回復(セルレギオス武器は7回復)。ボウガンは弾1発装填。50%の確率で装填数+1。弓は接撃ビンのダメージが1.5倍(セルレギオス武器は1.65倍)</t>
-  </si>
-  <si>
-    <t>睡眠</t>
-  </si>
-  <si>
-    <t>睡眠無効/睡眠倍加</t>
-  </si>
-  <si>
-    <t>睡眠状態にならなくなる/睡眠状態の時間が2倍になる</t>
-  </si>
-  <si>
-    <t>睡眠瓶追加</t>
-  </si>
-  <si>
-    <t>睡眠ビン追加</t>
-  </si>
-  <si>
-    <t>睡眠ビンの装着が可能になる</t>
-  </si>
-  <si>
-    <t>スタミナ</t>
-  </si>
-  <si>
-    <t>ランナー/鈍足</t>
-  </si>
-  <si>
-    <t>ダッシュ、鬼人状態、突進、溜め時などのスタミナ消費量が1/2になる/ダッシュ、鬼人状態、突進、溜め時などのスタミナ消費量が1.2倍になる</t>
-  </si>
-  <si>
-    <t>青電主</t>
-  </si>
-  <si>
-    <t>青電主の魂</t>
-  </si>
-  <si>
-    <t>超会心 + 連発数+1 + 斬れ味レベル+1</t>
-  </si>
-  <si>
-    <t>精密射撃</t>
-  </si>
-  <si>
-    <t>ブレ抑制+2/ブレ抑制+1/ブレ抑制-1/ブレ抑制-2</t>
-  </si>
-  <si>
-    <t>弾道のブレ幅がなくなる/弾道のブレ幅が1段階減少する/弾道のブレ幅が1段階増加する/弾道のブレ幅がブレ大になる</t>
-  </si>
-  <si>
-    <t>隻眼</t>
-  </si>
-  <si>
-    <t>隻眼の魂</t>
-  </si>
-  <si>
-    <t>気絶無効 + 挑戦者+2</t>
-  </si>
-  <si>
-    <t>接撃瓶追加</t>
-  </si>
-  <si>
-    <t>接撃ビン追加</t>
-  </si>
-  <si>
-    <t>接撃ビンの装着が可能になる</t>
-  </si>
-  <si>
-    <t>節食</t>
-  </si>
-  <si>
-    <t>満足感</t>
-  </si>
-  <si>
-    <t>食べたり飲んだりするアイテムが25%の確率で消費しなくなる</t>
-  </si>
-  <si>
-    <t>千里眼</t>
-  </si>
-  <si>
-    <t>自動マーキング/探知</t>
-  </si>
-  <si>
-    <t>常に中型、大型モンスターの位置と向きと攻撃状態が表示される/ペイント時に中型、大型モンスターの位置と向きと攻撃状態が表示される。また、ペイントしてない時でも一定の確率で同様の効果が得られる</t>
-  </si>
-  <si>
-    <t>走行継続</t>
-  </si>
-  <si>
-    <t>キープラン</t>
-  </si>
-  <si>
-    <t>スタミナ残り25(ゲージ赤色)以下でスタミナ消費と速度低下が無くなりダッシュし続けられる。</t>
-  </si>
-  <si>
-    <t>装填数</t>
-  </si>
-  <si>
-    <t>装填数UP</t>
-  </si>
-  <si>
-    <t>ボウガンの装填数や、弓の溜め段階が1つ増加する(最大4段階まで)。ガンランスの砲撃やチャージアックスの装填数も増える</t>
-  </si>
-  <si>
-    <t>装填速度</t>
-  </si>
-  <si>
-    <t>装填速度+3/装填速度+2/装填速度+1/装填速度-1/装填速度-2/装填速度-3</t>
-  </si>
-  <si>
-    <t>ボウガンのリロードが3段階分速くなる。しゃがみ撃ちには影響なし。弓のビンが切り替えるだけで自動で装着される/ボウガンのリロードが2段階分速くなる。しゃがみ撃ちには影響なし。弓のビンが切り替えるだけで自動で装着される/ボウガンのリロードが1段階分速くなる。しゃがみ撃ちには影響なし。弓のビンの切り替えが0.75倍に速くなる/ボウガンのリロードが1段階分遅くなる。しゃがみ撃ちには影響なし。弓のビンの装着速度が1.1倍に遅くなる/ボウガンのリロードが2段階分遅くなる。しゃがみ撃ちには影響なし。弓のビンの装着速度が1.2倍に遅くなる/ボウガンのリロードが3段階分遅くなる。しゃがみ撃ちには影響なし。弓のビンの装着速度が1.3倍に遅くなる</t>
-  </si>
-  <si>
-    <t>増幅</t>
-  </si>
-  <si>
-    <t>属物強化</t>
-  </si>
-  <si>
-    <t>属性攻撃強化 + アイテム使用強化</t>
-  </si>
-  <si>
-    <t>属強瓶追加</t>
-  </si>
-  <si>
-    <t>属強ビン全LV追加/属強ビンLV1追加</t>
-  </si>
-  <si>
-    <t>全LVの属強ビンが使えるようになる/属強ビンLV1の装着が可能になる</t>
-  </si>
-  <si>
-    <t>速射</t>
-  </si>
-  <si>
-    <t>連発数+1</t>
-  </si>
-  <si>
-    <t>速射時の発射数が+1される</t>
-  </si>
-  <si>
-    <t>属性会心</t>
-  </si>
-  <si>
-    <t>会心撃【属性】</t>
-  </si>
-  <si>
-    <t>クリティカル攻撃の際に与える属性ダメージ(火、水、雷、氷、龍)を高める。大剣は1.2倍。ボウガンは1.3倍。片手剣、双剣、弓は1.35倍。その他は1.25倍</t>
-  </si>
-  <si>
-    <t>属性攻撃</t>
-  </si>
-  <si>
-    <t>属性攻撃強化/属性攻撃弱化</t>
-  </si>
-  <si>
-    <t>火、水、雷、氷、龍の属性値が1.1倍になる。/火、水、雷、氷、龍の属性値が0.9倍になる</t>
-  </si>
-  <si>
-    <t>属性耐性</t>
-  </si>
-  <si>
-    <t>属性やられ無効</t>
-  </si>
-  <si>
-    <t>火、水、雷、氷、龍の属性やられにならなくなる</t>
-  </si>
-  <si>
-    <t>底力</t>
-  </si>
-  <si>
-    <t>火事場力+2/火事場力+1/心配性</t>
-  </si>
-  <si>
-    <t>体力が40%以下になると防御力が45増加。攻撃力1.3倍/体力が40%以下になると防御力が45増加。/体力が40%以下になると防御力が+30から+21に減少。攻撃力0.7倍</t>
-  </si>
-  <si>
-    <t>対炎龍</t>
-  </si>
-  <si>
-    <t>鋼殻の護り</t>
-  </si>
-  <si>
-    <t>南風の狩人 + 火耐性【大】 + 細菌研究家</t>
-  </si>
-  <si>
-    <t>対霞龍</t>
-  </si>
-  <si>
-    <t>炎鱗の護り</t>
-  </si>
-  <si>
-    <t>毒耐性 + 盗み無効 + 自動マーキング</t>
-  </si>
-  <si>
-    <t>耐寒</t>
-  </si>
-  <si>
-    <t>寒さ無効/寒さ倍加</t>
-  </si>
-  <si>
-    <t>寒さによるスタミナ減少を無効化する/寒さによるスタミナ減少が倍加する</t>
-  </si>
-  <si>
-    <t>対鋼龍</t>
-  </si>
-  <si>
-    <t>霞皮の護り</t>
-  </si>
-  <si>
-    <t>北風の狩人 + 風圧【大】無効 + だるま無効</t>
-  </si>
-  <si>
-    <t>体術</t>
-  </si>
-  <si>
-    <t>体術+2/体術+1/体術-1/体術-2</t>
-  </si>
-  <si>
-    <t>回避とガード時などのスタミナ消費が半分になる。大型モンスターに向かって緊急回避ができるようになり、緊急回避の移動距離が伸びる/回避とガード時などのスタミナ消費が0.75倍になる。大型モンスターに向かって緊急回避ができるようになり、緊急回避の移動距離が伸びる/回避とガード時などのスタミナ消費が1.2倍に増加する/回避とガード時などのスタミナ消費が1.35倍に増加する</t>
-  </si>
-  <si>
-    <t>耐暑</t>
-  </si>
-  <si>
-    <t>暑さ無効/暑さ倍加</t>
-  </si>
-  <si>
-    <t>暑さ、溶岩地形、炎まといによるダメージを無効化する/暑さ、溶岩地形、炎まといによるダメージが倍加する</t>
-  </si>
-  <si>
-    <t>耐震</t>
-  </si>
-  <si>
-    <t>振動によるふらつき状態を無効化</t>
-  </si>
-  <si>
-    <t>対防御DOWN</t>
-  </si>
-  <si>
-    <t>鉄面皮</t>
-  </si>
-  <si>
-    <t>防御力DOWN状態を無効化</t>
-  </si>
-  <si>
-    <t>体力</t>
-  </si>
-  <si>
-    <t>体力+50/体力+20/体力-10/体力-30</t>
-  </si>
-  <si>
-    <t>体力最大値+50/体力最大値+20/体力最大値-10/体力最大値-30</t>
-  </si>
-  <si>
-    <t>宝纏</t>
-  </si>
-  <si>
-    <t>宝纏の魂</t>
-  </si>
-  <si>
-    <t>お守りハンター + 腹減り無効</t>
-  </si>
-  <si>
-    <t>匠</t>
-  </si>
-  <si>
-    <t>斬れ味レベル+2/斬れ味レベル+1</t>
-  </si>
-  <si>
-    <t>斬れ味ゲージが2段階伸びる/斬れ味ゲージが1段階伸びる</t>
-  </si>
-  <si>
-    <t>茸食</t>
-  </si>
-  <si>
-    <t>キノコ大好き</t>
-  </si>
-  <si>
-    <t>キノコを食べることで有効な効果を得られる。アオキノコ：回復薬、ニトロダケとドスマツタケ：鬼人薬、マヒダケとオオマヒシメジ：硬化薬、毒テングダケ：栄養剤、ドキドキノコ：ランダムだが悪い効果は出ない、クタビレダケ：強走薬、厳選キノコ：強走薬グレート、マンドラゴラ：秘薬、特産キノコ：携帯食料、熟成キノコ：いにしえの秘薬、深層シメジ：ウチケシの実、コシカケダケ：解毒薬、混沌茸：千里眼の薬</t>
-  </si>
-  <si>
-    <t>達人</t>
-  </si>
-  <si>
-    <t>見切り+3/見切り+2/見切り+1/見切り-1/見切り-2/見切り-3</t>
-  </si>
-  <si>
-    <t>会心率+30%/会心率+20%/会心率+10%/会心率-5%/会心率-10%/会心率-15%</t>
-  </si>
-  <si>
-    <t>盾持</t>
-  </si>
-  <si>
-    <t>盾使い</t>
-  </si>
-  <si>
-    <t>ガード強化 + スタミナ急速回復</t>
+    <t>신멸인(燼滅刃)</t>
+  </si>
+  <si>
+    <t>신멸인의 혼(燼滅刃の魂)</t>
+  </si>
+  <si>
+    <t>예리도 레벨+2(斬れ味レベル+2) + 탄도강화(弾導強化) + 숫돌 사용 고속화(砥石使用高速化)</t>
+  </si>
+  <si>
+    <t>진・개열(真・鎧裂)</t>
+  </si>
+  <si>
+    <t>진・개열의 혼(真・鎧裂の魂)</t>
+  </si>
+  <si>
+    <t>가드 성능+2(ガード性能+2) + 납도술(納刀術) + 인린연마(刃鱗磨き)</t>
+  </si>
+  <si>
+    <t>인린(刃鱗)</t>
+  </si>
+  <si>
+    <t>인린연마(刃鱗磨き)</t>
+  </si>
+  <si>
+    <t>발도중에 회피행동에 의해 효과발동. 검사는 예리도 5회복(셀레기오스 무기는 7회복). 보우건은 탄 1발 장전. 50%의 확률로 장전수+1. 활은 접격병의 데미지가 1.5배(셀레기오스 무기는 1.65배)</t>
+  </si>
+  <si>
+    <t>수면(睡眠)</t>
+  </si>
+  <si>
+    <t>수면무효(睡眠無効)/수면배가(睡眠倍加)</t>
+  </si>
+  <si>
+    <t>수면상태 무효화/수면상태의 시간이 2배가 된다.</t>
+  </si>
+  <si>
+    <t>수면병추가(睡眠瓶追加)</t>
+  </si>
+  <si>
+    <t>수면병 추가(睡眠ビン追加)</t>
+  </si>
+  <si>
+    <t>수면병의 장착이 가능하게 된다.</t>
+  </si>
+  <si>
+    <t>스태미너(スタミナ)</t>
+  </si>
+  <si>
+    <t>러너(ランナー)/둔족(鈍足)</t>
+  </si>
+  <si>
+    <t>대시, 귀인상태, 돌진, 차지 등의 스태미너 소비량이 1/2이 된다./대시, 귀인상태, 돌진, 차지 등의 스태미너 소비량이 1.2배가 된다.</t>
+  </si>
+  <si>
+    <t>청전주(青電主)</t>
+  </si>
+  <si>
+    <t>청전주의 혼(青電主の魂)</t>
+  </si>
+  <si>
+    <t>초회심(超会心) + 연발수+1(連発数+1) + 예리도 레벨+1(斬れ味レベル+1)</t>
+  </si>
+  <si>
+    <t>정밀사격(精密射撃)</t>
+  </si>
+  <si>
+    <t>흔들림 억제+2(ブレ抑制+2)/흔들림 억제+1(ブレ抑制+1)/흔들림 억제-1(ブレ抑制-1)/흔들림 억제-2(ブレ抑制-2)</t>
+  </si>
+  <si>
+    <t>탄도의 흔들림 폭이 없어짐/탄도의 흔들림 폭이 1단계 감소한다./탄도의 흔들림 폭이 1단계 증가됨/탄도의 흔들림 폭이 대가 됨</t>
+  </si>
+  <si>
+    <t>척안(隻眼)</t>
+  </si>
+  <si>
+    <t>척안의 혼(隻眼の魂)</t>
+  </si>
+  <si>
+    <t>기절무효(気絶無効) + 도전자+2(挑戦者+2)</t>
+  </si>
+  <si>
+    <t>접격병추가(接撃瓶追加)</t>
+  </si>
+  <si>
+    <t>접격병 추가(接撃ビン追加)</t>
+  </si>
+  <si>
+    <t>접격병의 장착이 가능하게 된다.</t>
+  </si>
+  <si>
+    <t>절식(節食)</t>
+  </si>
+  <si>
+    <t>만족감(満足感)</t>
+  </si>
+  <si>
+    <t>먹거나 마시는 아이템이 25%의 확률로 소비하지 않게 된다.</t>
+  </si>
+  <si>
+    <t>천리안(千里眼)</t>
+  </si>
+  <si>
+    <t>자동 마킹(自動マーキング)/탐지(探知)</t>
+  </si>
+  <si>
+    <t>항상 중형, 대형 몬스터의 위치와 방향과 공격상태가 표시된다./페인트 시에 중형, 대형 몬스터의 위치와 방향과 공격상태가 표시된다. 또, 페인트 하지 않았을 때도 일정 확률로 같은 효과를 얻을 수 있다.</t>
+  </si>
+  <si>
+    <t>주행계속(走行継続)</t>
+  </si>
+  <si>
+    <t>킵 런(キープラン)</t>
+  </si>
+  <si>
+    <t>스태미너 잔량이 25(게이지 적색)이하에서 스태미너 소비와 속도저하가 없어지고 대시를 계속할 수 있게 된다.</t>
+  </si>
+  <si>
+    <t>장전수(装填数)</t>
+  </si>
+  <si>
+    <t>장전수UP(装填数UP)</t>
+  </si>
+  <si>
+    <t>보우건의 장전수나 활의 차지 단계가 하나 증가된다(최대 4단계까지). 건랜스의 포격이나 차지 액스의 장전수도 늘어난다.</t>
+  </si>
+  <si>
+    <t>장전속도(装填速度)</t>
+  </si>
+  <si>
+    <t>장전속도+3(装填速度+3)/장전속도+2(装填速度+2)/장전속도+1(装填速度+1)/장전속도-1(装填速度-1)/장전속도-2(装填速度-2)/장전속도-3(装填速度-3)</t>
+  </si>
+  <si>
+    <t>보우건의 리로드가 3단계 빨라짐. 앉아쏘기에는 영향없음. 활의 병이 교체하는 것만으로 자동으로 장전됨/보우건의 리로드가 2단계 빨라짐. 앉아쏘기에는 영향없음. 활의 병이 교체하는 것만으로 자동으로 장전됨./보우건의 리로드가 1단계 빨라짐. 앉아쏘기에는 영향 없음. 활의 병 교체시간이 0.75배로 빨라짐/보우건의 리로드가 1단계 느려짐. 앉아쏘기에는 영향없음. 활의 병 교체시간이 1.1배로 느려짐/보우건의 리로드가 2단계 느려짐. 앉아쏘기에는 영향없음. 활의 병 교체시간이 1.2배로 느려짐/보우건의 리로드가 3단계 느려짐. 앉아쏘기에는 영향없음. 활의 병 교체시간이 1.3배로 느려짐.</t>
+  </si>
+  <si>
+    <t>증폭(増幅)</t>
+  </si>
+  <si>
+    <t>증폭강화(属物強化)</t>
+  </si>
+  <si>
+    <t>강속성 공격(属性攻撃強化) + 아이템 사용 강화(アイテム使用強化)</t>
+  </si>
+  <si>
+    <t>속강병추가(属強瓶追加)</t>
+  </si>
+  <si>
+    <t>강속병 전LV 추가(属強ビン全LV追加)/강속병 LV1 추가(属強ビンLV1追加)</t>
+  </si>
+  <si>
+    <t>전LV의 강속병을 사용할 수 있게 된다./강속병 LV1의 장착이 가능하게 된다.</t>
+  </si>
+  <si>
+    <t>속사(速射)</t>
+  </si>
+  <si>
+    <t>연발수+1(連発数+1)</t>
+  </si>
+  <si>
+    <t>속사시의 연발수가+1 된다.</t>
+  </si>
+  <si>
+    <t>속성회심(属性会心)</t>
+  </si>
+  <si>
+    <t>회심격【속성】(会心撃【属性】)</t>
+  </si>
+  <si>
+    <t>크리티컬 공격 시 가하는 속성 데미지(화, 수, 뇌, 빙, 용)를 높힌다. 대검은 1.2배.  보우건은 1.3배. 한손검, 쌍검, 활은 1.35배. 그 외는 1.25배</t>
+  </si>
+  <si>
+    <t>속성공격(属性攻撃)</t>
+  </si>
+  <si>
+    <t>속성공격강화(属性攻撃強化)/속성공격약화(属性攻撃弱化)</t>
+  </si>
+  <si>
+    <t>화, 수, 뇌, 빙, 용의 속성치가 1.1배가 된다./화, 수, 뇌, 빙, 용의 속성치가 0.9가 된다.</t>
+  </si>
+  <si>
+    <t>속성내성(属性耐性)</t>
+  </si>
+  <si>
+    <t>속성 피해 무효(属性やられ無効)</t>
+  </si>
+  <si>
+    <t>화, 수, 뇌, 빙, 용의 속성 피해 무효화</t>
+  </si>
+  <si>
+    <t>저력(底力)</t>
+  </si>
+  <si>
+    <t>화사장력+2(火事場力+2)/화사장력+1(火事場力+1)/걱정이태산(心配性)</t>
+  </si>
+  <si>
+    <t>체력이 40%이하가 되면 방어력이 45증가. 공격력 1.3배/체력이 40%이하가 되면 방어력이 45증가./체력이 40%이하가 되면 방어력이 +30에서 +21로 감소. 공격력 0.7배</t>
+  </si>
+  <si>
+    <t>대염룡(対炎龍)</t>
+  </si>
+  <si>
+    <t>강각의 수호(鋼殻の護り)</t>
+  </si>
+  <si>
+    <t>남풍의 사냥꾼(南風の狩人) + 화내성【대】(火耐性【大】) + 세균 연구가(細菌研究家)</t>
+  </si>
+  <si>
+    <t>대하룡(対霞龍)</t>
+  </si>
+  <si>
+    <t>염린의 수호(炎鱗の護り)</t>
+  </si>
+  <si>
+    <t>독내성(毒耐性) + 도난 무효(盗み無効) + 자동 마킹(自動マーキング)</t>
+  </si>
+  <si>
+    <t>내한(耐寒)</t>
+  </si>
+  <si>
+    <t>추위 무효(寒さ無効)/추위 배가(寒さ倍加)</t>
+  </si>
+  <si>
+    <t>추위에 의한 스태미너 감소를 무효화한다./추위에 의한 스태미너 감소가 배가된다.</t>
+  </si>
+  <si>
+    <t>대강룡(対鋼龍)</t>
+  </si>
+  <si>
+    <t>하피의 수호(霞皮の護り)</t>
+  </si>
+  <si>
+    <t>북풍의 사냥꾼(北風の狩人) + 풍압【대】 무효(風圧【大】無効) + 눈사람 무효(だるま無効)</t>
+  </si>
+  <si>
+    <t>체술(体術)</t>
+  </si>
+  <si>
+    <t>체술+2(体術+2)/체술+1(体術+1)/체술-1(体術-1)/체술-2(体術-2)</t>
+  </si>
+  <si>
+    <t>회피와 가드 등의 스태미너 소비가 절반이 된다. 대형 몬스터를 향해 긴급회피가 가능하게 되고 긴급회피의 이동거리가 늘어난다./회피와 가드 등의 스태미너 소비가 0.75배가 된다. 대형 몬스터를 향해 긴급회피가 가능하게 되고 긴급회피의 이동거리가 늘어난다./회피와 가드 등의 스태미너 소비가 1.2배로 증가한다./회피와 가드 등의 스태미너 소비가 1.35배로 증가한다.</t>
+  </si>
+  <si>
+    <t>내서(耐暑)</t>
+  </si>
+  <si>
+    <t>더위 무효(暑さ無効)/더위 배가(暑さ倍加)</t>
+  </si>
+  <si>
+    <t>더위, 용암지형, 불길에 의한 데미지를 무효화한다./더위, 용암지형, 불길에 의한 데미지가 배가된다.</t>
+  </si>
+  <si>
+    <t>내진(耐震)</t>
+  </si>
+  <si>
+    <t>진동에 의해 휘청거리는 상태를 무효화</t>
+  </si>
+  <si>
+    <t>방어력DOWN(対防御DOWN)</t>
+  </si>
+  <si>
+    <t>철면피(鉄面皮)</t>
+  </si>
+  <si>
+    <t>방어력DOWN상태를 무효화</t>
+  </si>
+  <si>
+    <t>체력(体力)</t>
+  </si>
+  <si>
+    <t>체력+50(体力+50)/체력+20(体力+20)/체력-10(体力-10)/체력-30(体力-30)</t>
+  </si>
+  <si>
+    <t>체력 최대치+50/체력 최대치+20/체력 최대치-10/체력 최대치-30</t>
+  </si>
+  <si>
+    <t>보전(宝纏)</t>
+  </si>
+  <si>
+    <t>보전의 혼(宝纏の魂)</t>
+  </si>
+  <si>
+    <t>부적 헌터(お守りハンター) + 배고픔 무효(腹減り無効)</t>
+  </si>
+  <si>
+    <t>장(匠)</t>
+  </si>
+  <si>
+    <t>예리도 레벨+2(斬れ味レベル+2)/예리도 레벨+1(斬れ味レベル+1)</t>
+  </si>
+  <si>
+    <t>예리도 게이지가 2단계 늘어난다./예리도 게이지가 1단계 늘어난다.</t>
+  </si>
+  <si>
+    <t>이식(茸食)</t>
+  </si>
+  <si>
+    <t>버섯 애호가(キノコ大好き)</t>
+  </si>
+  <si>
+    <t>버섯을 먹는 것으로 유효한 효과를 얻을 수 있다. 파란 버섯(アオキノコ)：회복약, 니트로 버섯(ニトロダケ)과 도스 송이버섯(ドスマツタケ)：귀인약, 마비버섯(マヒダケ)과 큰 마비 시메지(オオマヒシメジ)：경화약, 독광대 버섯(毒テングダケ)：영양제, 두근두근 버섯(ドキドキノコ)：랜덤이지만 나쁜 효과는 나오지 않음, 녹초버섯(クタビレダケ)：강주약, 엄선 버섯(厳選キノコ)：강주약 그레이트, 만드라고라(マンドラゴラ)：비약, 특산 버섯(特産キノコ)：휴대용 식량, 숙성 버섯(熟成キノコ)：고대의 비약, 심층 시메지(深層シメジ)：지움 열매, 걸상 버섯(コシカケダケ)：해독약, 혼돈 버섯(混沌茸)：천리안의 약</t>
+  </si>
+  <si>
+    <t>달인(達人)</t>
+  </si>
+  <si>
+    <t>간파+3(見切り+3)/간파+2(見切り+2)/간파+1(見切り+1)/간파-1(見切り-1)/간파-2(見切り-2)/간파-3(見切り-3)</t>
+  </si>
+  <si>
+    <t>회심률+30%/회심률+20%/회심률+10%/회심률-5%/회심률-10%/회심률-15%</t>
+  </si>
+  <si>
+    <t>순지(盾持)</t>
+  </si>
+  <si>
+    <t>방패사용(盾使い)</t>
+  </si>
+  <si>
+    <t>가드 강화(ガード強化) + 스태미너 급속회복(スタミナ急速回復)</t>
   </si>
   <si>
     <t>溜め短縮</t>
@@ -2260,8 +2260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C86" workbookViewId="0">
-      <selection activeCell="D103" sqref="D103"/>
+    <sheetView tabSelected="1" topLeftCell="D129" workbookViewId="0">
+      <selection activeCell="D140" sqref="D140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Skill information translation. (~170)
</commit_message>
<xml_diff>
--- a/skill.xlsx
+++ b/skill.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19120"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19125"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
@@ -1204,7 +1204,7 @@
     <t>하피의 수호(霞皮の護り)</t>
   </si>
   <si>
-    <t>북풍의 사냥꾼(北風の狩人) + 풍압【대】 무효(風圧【大】無効) + 눈사람 무효(だるま無効)</t>
+    <t>북풍의 사냥꾼(北風の狩人) + 풍압【대】 무효(風圧【大】無効) + 오뚝이 무효(だるま無効)</t>
   </si>
   <si>
     <t>체술(体術)</t>
@@ -1294,268 +1294,268 @@
     <t>가드 강화(ガード強化) + 스태미너 급속회복(スタミナ急速回復)</t>
   </si>
   <si>
-    <t>溜め短縮</t>
-  </si>
-  <si>
-    <t>集中/雑念</t>
-  </si>
-  <si>
-    <t>大剣、ハンマー、弓の溜め時間が0.8倍になり、太刀、双剣、スラッシュアックス、チャージアックスのゲージが溜まりが1.2倍になる。/大剣、ハンマー、弓の溜め時間が1.2倍になり、太刀、双剣、スラッシュアックス、チャージアックスのゲージが溜まりが0.8倍になる。</t>
-  </si>
-  <si>
-    <t>だるま</t>
-  </si>
-  <si>
-    <t>だるま無効</t>
-  </si>
-  <si>
-    <t>雪だるま状態、泡状態【大】、骨まみれ状態を無効化</t>
-  </si>
-  <si>
-    <t>弾薬節約</t>
-  </si>
-  <si>
-    <t>射撃時に20%の確率で弾やビンを消費しない</t>
-  </si>
-  <si>
-    <t>チャンス</t>
-  </si>
-  <si>
-    <t>切り札</t>
-  </si>
-  <si>
-    <t>同エリアの大型モンスターがやられ、ダウンした際に1分間狩技のダメージと効果時間が1.2倍になる。それ以外にも一部の狩技の効果が上がる</t>
-  </si>
-  <si>
-    <t>聴覚保護</t>
-  </si>
-  <si>
-    <t>高級耳栓/耳栓</t>
-  </si>
-  <si>
-    <t>咆哮【小】と咆哮【大】を無効化。ダメージ有りの咆哮は防げない/咆哮【小】を無効化</t>
-  </si>
-  <si>
-    <t>調合数</t>
-  </si>
-  <si>
-    <t>最大数生産</t>
-  </si>
-  <si>
-    <t>調合の生産数が必ず最大になる</t>
-  </si>
-  <si>
-    <t>調合成功率</t>
-  </si>
-  <si>
-    <t>調合成功率+45%/調合成功率+20%/調合成功率-10%/調合成功率-20%</t>
-  </si>
-  <si>
-    <t>調合の成功率+45%/調合の成功率+20%/調合の成功率-10%/調合の成功率-20%</t>
-  </si>
-  <si>
-    <t>跳躍</t>
-  </si>
-  <si>
-    <t>飛燕</t>
-  </si>
-  <si>
-    <t>ジャンプ攻撃時の威力と乗り属性蓄積値、ダウン属性蓄積値が1.1倍にアップ</t>
-  </si>
-  <si>
-    <t>痛撃</t>
-  </si>
-  <si>
-    <t>弱点特効</t>
-  </si>
-  <si>
-    <t>攻撃時に肉質が45%以上だと会心率に+50%の補正が付いてダメージを与える</t>
-  </si>
-  <si>
-    <t>通常弾強化</t>
-  </si>
-  <si>
-    <t>通常弾・連射矢UP</t>
-  </si>
-  <si>
-    <t>通常弾、連射矢の威力が1.1倍になる</t>
-  </si>
-  <si>
-    <t>通常弾追加</t>
-  </si>
-  <si>
-    <t>通常弾全LV追加</t>
-  </si>
-  <si>
-    <t>全LVの通常弾が使えるようになる</t>
-  </si>
-  <si>
-    <t>天眼</t>
-  </si>
-  <si>
-    <t>天眼の魂</t>
-  </si>
-  <si>
-    <t>見切り+3 + 挑戦者+1</t>
-  </si>
-  <si>
-    <t>胴系統倍加</t>
+    <t>차지단축(溜め短縮)</t>
+  </si>
+  <si>
+    <t>집중(集中)/잡념(雑念)</t>
+  </si>
+  <si>
+    <t>대검, 해머, 활의 차지 시간이 0.8배가 되고 태도, 쌍검, 슬래시 액스, 챠지 액스의 게이지 충전량이 1.2배가 된다./대검, 해머, 활의 차지 시간이 1.2배가 되고 태도, 쌍검, 슬래시 액스, 챠지 액스의 게이지 충전량이 0.8배가 된다.</t>
+  </si>
+  <si>
+    <t>오뚝이(だるま)</t>
+  </si>
+  <si>
+    <t>오뚝이 무효(だるま無効)</t>
+  </si>
+  <si>
+    <t>눈사람 상태, 거품 상태【대】, 뼈 투성이 상태를 무효화</t>
+  </si>
+  <si>
+    <t>탄약절약(弾薬節約)</t>
+  </si>
+  <si>
+    <t>사격 시에 20%의 확률로 탄이나 병을 소모하지 않는다.</t>
+  </si>
+  <si>
+    <t>찬스(チャンス)</t>
+  </si>
+  <si>
+    <t>비장의 카드(切り札)</t>
+  </si>
+  <si>
+    <t>같은 에어리어의 대형 몬스터가 당함, 다운했을 때에 1분간 수기의 게이지와 효과시간이 1.2배가 된다. 그 이외에도 일부 수기의 효과가 상승한다.</t>
+  </si>
+  <si>
+    <t>청각보호(聴覚保護)</t>
+  </si>
+  <si>
+    <t>고급 귀마개(高級耳栓)/귀마개(耳栓)</t>
+  </si>
+  <si>
+    <t>포효【소】와 포효【대】를 무효화. 데미지가 있는 포효는 막을 수 없다./포효【소】를 무효화</t>
+  </si>
+  <si>
+    <t>조합수(調合数)</t>
+  </si>
+  <si>
+    <t>최대수생산(最大数生産)</t>
+  </si>
+  <si>
+    <t>조합의 생산수가 반드시 최대가 된다.</t>
+  </si>
+  <si>
+    <t>조합성공률(調合成功率)</t>
+  </si>
+  <si>
+    <t>조합성공률+45%(調合成功率+45%)/조합성공률+20%(調合成功率+20%)/조합성공률-10%(調合成功率-10%)/조합성공률-20%(調合成功率-20%)</t>
+  </si>
+  <si>
+    <t>조합 성공률+45%/조합 성공률+20%/조합 성공률-10%/조합 성공률-20%</t>
+  </si>
+  <si>
+    <t>도약(跳躍)</t>
+  </si>
+  <si>
+    <t>비연(飛燕)</t>
+  </si>
+  <si>
+    <t>점프 공격시에 위력과 단차 속성축적치, 다운 속성축적치가 1.1배로 상승</t>
+  </si>
+  <si>
+    <t>통격(痛撃)</t>
+  </si>
+  <si>
+    <t>약점특효(弱点特効)</t>
+  </si>
+  <si>
+    <t>공격시에 육질이 45%이상이면 회심률에 50%의 보정이 붙는다.</t>
+  </si>
+  <si>
+    <t>통상탄 강화(通常弾強化)</t>
+  </si>
+  <si>
+    <t>통상탄・연사 화살UP(通常弾・連射矢UP)</t>
+  </si>
+  <si>
+    <t>통상탄, 연사 화살의 위력이 1.1배가 된다.</t>
+  </si>
+  <si>
+    <t>통상탄추가(通常弾追加)</t>
+  </si>
+  <si>
+    <t>통상탄 전LV 추가(通常弾全LV追加)</t>
+  </si>
+  <si>
+    <t>전LV의 통상탄을 사용할 수 있게 된다.</t>
+  </si>
+  <si>
+    <t>천안(天眼)</t>
+  </si>
+  <si>
+    <t>천안의 혼(天眼の魂)</t>
+  </si>
+  <si>
+    <t>간파+3(見切り+3) + 도전자+1(挑戦者+1)</t>
+  </si>
+  <si>
+    <t>몸통 배가(胴系統倍加)</t>
   </si>
   <si>
     <t>0</t>
   </si>
   <si>
-    <t>胴パーツのスキルポイントが2倍になる</t>
-  </si>
-  <si>
-    <t>闘魂</t>
-  </si>
-  <si>
-    <t>挑戦者+2/挑戦者+1</t>
-  </si>
-  <si>
-    <t>大型モンスターの怒りに反応して3秒後に攻撃力が20、会心率が15%上がる。スキルの力の解放、フルチャージとは重複しない/大型モンスターの怒りに反応して3秒後に攻撃力が10、会心率が10%上がる。スキルの力の解放、フルチャージとは重複しない</t>
-  </si>
-  <si>
-    <t>刀匠</t>
-  </si>
-  <si>
-    <t>真打</t>
-  </si>
-  <si>
-    <t>斬れ味レベル+1 + 攻撃力UP【大】</t>
-  </si>
-  <si>
-    <t>研ぎ師</t>
-  </si>
-  <si>
-    <t>砥石使用高速化/砥石使用低速化</t>
-  </si>
-  <si>
-    <t>砥石系アイテム研ぎ時間が短くなる。通常の4回から1回になる。/砥石系アイテム研ぎ時間が長くなる。通常の4回から5回になる。</t>
-  </si>
-  <si>
-    <t>毒</t>
-  </si>
-  <si>
-    <t>毒耐性/毒倍加</t>
-  </si>
-  <si>
-    <t>毒、猛毒状態にならない。劇毒は猛毒に軽減される/毒によって受けるダメージが2倍になる</t>
-  </si>
-  <si>
-    <t>特殊会心</t>
-  </si>
-  <si>
-    <t>会心撃【特殊】</t>
-  </si>
-  <si>
-    <t>クリティカル攻撃の際に与える状態異常値(麻痺、毒、睡眠)が1.2倍になる</t>
-  </si>
-  <si>
-    <t>特殊攻撃</t>
-  </si>
-  <si>
-    <t>状態異常攻撃+2/状態異常攻撃+1/状態異常攻撃弱化</t>
-  </si>
-  <si>
-    <t>毒、麻痺、睡眠、捕獲麻酔の属性値が1.2倍+1になる/毒、麻痺、睡眠、捕獲麻酔の属性値が1.1倍+1になる/毒、麻痺、睡眠、捕獲麻酔の属性値が0.9倍になる</t>
-  </si>
-  <si>
-    <t>毒瓶追加</t>
-  </si>
-  <si>
-    <t>毒ビン追加</t>
-  </si>
-  <si>
-    <t>毒ビンの装着が可能になる</t>
-  </si>
-  <si>
-    <t>鈍器</t>
-  </si>
-  <si>
-    <t>鈍器使い</t>
-  </si>
-  <si>
-    <t>斬れ味が悪いほど攻撃力アップ。ゲージが緑：1.1倍、黄：1.15倍、橙、赤：1.2倍</t>
-  </si>
-  <si>
-    <t>肉食</t>
-  </si>
-  <si>
-    <t>お肉大好き</t>
-  </si>
-  <si>
-    <t>生肉が食べられるようになりスタミナの最大値が50上がる。また、生焼け肉やこんがり肉、クーラーミート、ホットミートで1分間強走効果がつく</t>
-  </si>
-  <si>
-    <t>盗み無効</t>
-  </si>
-  <si>
-    <t>アイテムを盗まれなくなる</t>
-  </si>
-  <si>
-    <t>納刀</t>
-  </si>
-  <si>
-    <t>納刀術</t>
-  </si>
-  <si>
-    <t>武器を納める速度が1.4倍になる</t>
-  </si>
-  <si>
-    <t>納刀研磨</t>
-  </si>
-  <si>
-    <t>挑戦者の納刀</t>
-  </si>
-  <si>
-    <t>モンスターが怒り状態のときに納刀すると、25%の確率で斬れ味が回復。回復量は武器種により異なる。</t>
-  </si>
-  <si>
-    <t>乗り</t>
-  </si>
-  <si>
-    <t>乗り名人/乗り下手</t>
-  </si>
-  <si>
-    <t>乗り蓄積値が1.25倍に増え、乗り状態時の攻撃ゲージの増加量が1.25倍になる/乗り蓄積値が0.9倍に減り、乗り状態時の攻撃ゲージの増加量が0.9倍になる</t>
-  </si>
-  <si>
-    <t>剥ぎ取り</t>
-  </si>
-  <si>
-    <t>剥ぎ取り名人/剥ぎ取り鉄人</t>
-  </si>
-  <si>
-    <t>剥ぎ取り回数が1回増加し、剥ぎ取り中にのけぞらなくなる/剥ぎ取り中にのけぞらなくなる</t>
-  </si>
-  <si>
-    <t>爆弾強化</t>
-  </si>
-  <si>
-    <t>ボマー</t>
-  </si>
-  <si>
-    <t>爆弾のダメージが1.3倍になる。爆破属性の蓄積値が1.2倍になる(ネコの火薬術と併用で1.25倍上限)。爆弾調合成功率が100％になる</t>
-  </si>
-  <si>
-    <t>爆破瓶追加</t>
-  </si>
-  <si>
-    <t>爆破ビン追加</t>
-  </si>
-  <si>
-    <t>爆破ビンを装着可能にする</t>
-  </si>
-  <si>
-    <t>ハチミツ</t>
-  </si>
-  <si>
-    <t>ハニーハンター</t>
-  </si>
-  <si>
-    <t>ハチミツやロイヤルハニーが一度に2個採取できる</t>
+    <t>몸 파츠의 스킬 포인트가 2배가 된다.</t>
+  </si>
+  <si>
+    <t>투혼(闘魂)</t>
+  </si>
+  <si>
+    <t>도전자+2(挑戦者+2)/도전자+1(挑戦者+1)</t>
+  </si>
+  <si>
+    <t>대형 몬스터의 분노에 반응해서 3초후에 공격력이 20, 회심률이 15% 상승한다. 스킬 힘의해방(力の解放), 풀 챠지(フルチャージ)와는 중복되지 않는다./대형 몬스터의 분노에 반응해서 3초후에 공격력이 10, 회심률이 10% 상승한다. 스킬 힘의해방(力の解放), 풀 챠지(フルチャージ)와는 중복되지 않는다.</t>
+  </si>
+  <si>
+    <t>도장(刀匠)</t>
+  </si>
+  <si>
+    <t>진타(真打)</t>
+  </si>
+  <si>
+    <t>예리도 레벨+1(斬れ味レベル+1) + 공격력UP【대】(攻撃力UP【大】)</t>
+  </si>
+  <si>
+    <t>연마사(研ぎ師)</t>
+  </si>
+  <si>
+    <t>숫돌 사용 고속화(砥石使用高速化)/숫돌 사용 저속화(砥石使用低速化)</t>
+  </si>
+  <si>
+    <t>숫돌 계열 아이템의 연마 시간이 짧아진다. 통상의 4회에서 1회가 된다./숫돌 계열 아이템의 연마 시간이 길어진다. 통상의 4회에서 5회가 된다.</t>
+  </si>
+  <si>
+    <t>독(毒)</t>
+  </si>
+  <si>
+    <t>독내성(毒耐性)/독배가(毒倍加)</t>
+  </si>
+  <si>
+    <t>독, 맹독상태가 되지 않는다. 극독은 맹독으로 경감된다./독에 의해 받는 데미지가 2배가 된다.</t>
+  </si>
+  <si>
+    <t>특수회심(特殊会心)</t>
+  </si>
+  <si>
+    <t>회심격【특수】(会心撃【特殊】)</t>
+  </si>
+  <si>
+    <t>크리티컬 공격 시에 가하는 상태이상치(마비, 독, 수면)가 1.2배가 된다.</t>
+  </si>
+  <si>
+    <t>특수공격(特殊攻撃)</t>
+  </si>
+  <si>
+    <t>상태이상공격+2(状態異常攻撃+2)/상태이상공격+1(状態異常攻撃+1)/상태이상공격약화(状態異常攻撃弱化)</t>
+  </si>
+  <si>
+    <t>독, 마비, 수면, 포획마취의 속성치가 1.2배+1이 된다./독, 마비, 수면, 포획마취의 속성치가 1.1배+1이 된다./독, 마비, 수면, 포획마취의 속성치가 0.9배가 된다.</t>
+  </si>
+  <si>
+    <t>독병추가(毒瓶追加)</t>
+  </si>
+  <si>
+    <t>독병 추가(毒ビン追加)</t>
+  </si>
+  <si>
+    <t>독병의 장착이 가능하게 된다.</t>
+  </si>
+  <si>
+    <t>둔기(鈍器)</t>
+  </si>
+  <si>
+    <t>둔기사용(鈍器使い)</t>
+  </si>
+  <si>
+    <t>예리도가 나쁠수록 공격력 상승. 게이지가 녹색：1.1배, 황색：1.15배, 귤색이나 적색：1.2배</t>
+  </si>
+  <si>
+    <t>육식(肉食)</t>
+  </si>
+  <si>
+    <t>고기 애호가(お肉大好き)</t>
+  </si>
+  <si>
+    <t>생고기를 먹을 수 있게 되며 스태미너의 최대치가 50 상승한다. 또, 덜 익힌 고기나 탄 고기, 쿨 미트, 핫 미트로 1분간 강주효과가 발생.</t>
+  </si>
+  <si>
+    <t>도난 무효(盗み無効)</t>
+  </si>
+  <si>
+    <t>아이템을 도난당하지 않게 된다.</t>
+  </si>
+  <si>
+    <t>납도(納刀)</t>
+  </si>
+  <si>
+    <t>납도술(納刀術)</t>
+  </si>
+  <si>
+    <t>납도 속도가 1.4배가 된다.</t>
+  </si>
+  <si>
+    <t>납도연마(納刀研磨)</t>
+  </si>
+  <si>
+    <t>도전자의 납도(挑戦者の納刀)</t>
+  </si>
+  <si>
+    <t>몬스터가 분노 상태일 때 납도하면, 25%의 확률로 예리도가 회복. 회복량은 무기종류에 따라 다르다.</t>
+  </si>
+  <si>
+    <t>탑승(乗り)</t>
+  </si>
+  <si>
+    <t>탑승 명인(乗り名人)/탑승 하수(乗り下手)</t>
+  </si>
+  <si>
+    <t>탑승 축적치가 1.25배로 늘고, 탑승상태 시 공격 게이지의 증가량이 1.25배가 된다./탑승 축적치가 0.9배로 줄고, 탑승상태 시 공격 게이지의 증가량이 0.9배가 된다.</t>
+  </si>
+  <si>
+    <t>갈무리(剥ぎ取り)</t>
+  </si>
+  <si>
+    <t>갈무리 명인(剥ぎ取り名人)/갈무리 철인(剥ぎ取り鉄人)</t>
+  </si>
+  <si>
+    <t>갈무리 회수가 1회 증가하고, 갈무리 중에 움츠리지 않게 된다./갈무리 중에 움츠리지 않게 된다.</t>
+  </si>
+  <si>
+    <t>폭탄강화(爆弾強化)</t>
+  </si>
+  <si>
+    <t>보머(ボマー)</t>
+  </si>
+  <si>
+    <t>폭탄의 데미지가 1.3배가 된다. 폭파속성의 축적치가 1.2배가 된다(고양이 화약술과 병용해서 1.25배 상한). 폭탄 조합성공률이 100%가 된다.</t>
+  </si>
+  <si>
+    <t>폭파병추가(爆破瓶追加)</t>
+  </si>
+  <si>
+    <t>폭파병 추가(爆破ビン追加)</t>
+  </si>
+  <si>
+    <t>폭파병을 장착 가능하게 된다.</t>
+  </si>
+  <si>
+    <t>벌꿀(ハチミツ)</t>
+  </si>
+  <si>
+    <t>허니 헌터(ハニーハンター)</t>
+  </si>
+  <si>
+    <t>벌꿀(ハチミツ)이나 로열 허니(ロイヤルハニー)가 한 번에 2개 채취 가능하다.</t>
   </si>
   <si>
     <t>抜刀会心</t>
@@ -2260,8 +2260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D129" workbookViewId="0">
-      <selection activeCell="D140" sqref="D140"/>
+    <sheetView tabSelected="1" topLeftCell="D159" workbookViewId="0">
+      <selection activeCell="D170" sqref="D170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Skill information translation. (~End)
</commit_message>
<xml_diff>
--- a/skill.xlsx
+++ b/skill.xlsx
@@ -298,7 +298,7 @@
     <t>뇌내성【대】(雷耐性【大】)/뇌내성【소】(雷耐性【小】)/뇌내성 약화(雷耐性弱化)</t>
   </si>
   <si>
-    <t>뇌내성+20. 합계내성이 25이상이면 뇌속성 피해 소와 대를 무효화/뇌내성+15. 합계내성이 15이상이면 뇌속성 피해 소 무효화/뇌내성-20</t>
+    <t>뇌내성+20. 합계내성이 25이상이면 뇌속성 피해 소와 대를 무효화/뇌내성+15. 합계내성이 15이상이면 뇌속성 피해 소를 무효화/뇌내성-20</t>
   </si>
   <si>
     <t>사냥꾼(狩人)</t>
@@ -625,7 +625,7 @@
     <t>빙내성【대】(氷耐性【大】)/빙내성【소】(氷耐性【小】)/빙내성 약화(氷耐性弱化)</t>
   </si>
   <si>
-    <t>빙내성+20. 합계내성이 25이상이면 빙속성 피해 소와 대를 무효화/빙내성+15. 합계내성이 15이상이면 빙속성 피해 소 무효화/빙내성-20</t>
+    <t>빙내성+20. 합계내성이 25이상이면 빙속성 피해 소와 대를 무효화/빙내성+15. 합계내성이 15이상이면 빙속성 피해 소를 무효화/빙내성-20</t>
   </si>
   <si>
     <t>흑염왕(黒炎王)</t>
@@ -1558,328 +1558,328 @@
     <t>벌꿀(ハチミツ)이나 로열 허니(ロイヤルハニー)가 한 번에 2개 채취 가능하다.</t>
   </si>
   <si>
-    <t>抜刀会心</t>
-  </si>
-  <si>
-    <t>抜刀術【技】</t>
-  </si>
-  <si>
-    <t>武器出し攻撃時に会心率が+100%増える</t>
-  </si>
-  <si>
-    <t>抜刀減気</t>
-  </si>
-  <si>
-    <t>抜刀術【力】</t>
-  </si>
-  <si>
-    <t>切断属性の武器出し攻撃時に攻撃力5と減気値15(双剣は5)が追加される。頭に攻撃時には気絶値30も追加</t>
-  </si>
-  <si>
-    <t>腹減り</t>
-  </si>
-  <si>
-    <t>腹減り無効/腹減り半減/腹減り倍加【小】/腹減り倍加【大】</t>
-  </si>
-  <si>
-    <t>腹減りによるスタミナ減少がなくなる/腹減りによるスタミナ減少が1/2になる/腹減りによるスタミナ減少速度が1.5倍に上がる/腹減りによるスタミナ減少速度が2倍に上がる</t>
-  </si>
-  <si>
-    <t>反動</t>
-  </si>
-  <si>
-    <t>反動軽減+3/反動軽減+2/反動軽減+1/反動軽減-1/反動軽減-2/反動軽減-3</t>
-  </si>
-  <si>
-    <t>ボウガンの反動が3段階小さくなる。速射の反動には効果がない/ボウガンの反動が2段階小さくなる。速射の反動には効果がない/ボウガンの反動が1段階小さくなる。速射の反動には効果がない/ボウガンの反動が1段階大きくなる。速射の反動には効果がない/ボウガンの反動が2段階大きくなる。速射の反動には効果がない/ボウガンの反動が3段階大きくなる。速射の反動には効果がない</t>
-  </si>
-  <si>
-    <t>飛行酒場</t>
-  </si>
-  <si>
-    <t>飛行酒場の心</t>
-  </si>
-  <si>
-    <t>KO術 + 笛吹き名人</t>
-  </si>
-  <si>
-    <t>秘術</t>
-  </si>
-  <si>
-    <t>スキル加点+2</t>
-  </si>
-  <si>
-    <t>装備しているスキルポイントの合計値に+2される。</t>
-  </si>
-  <si>
-    <t>火属性攻撃</t>
-  </si>
-  <si>
-    <t>火属性攻撃強化+2/火属性攻撃強化+1/火属性攻撃弱化</t>
-  </si>
-  <si>
-    <t>火属性の攻撃が1.1倍+6になる/火属性の攻撃が1.05倍+4になる/火属性の攻撃が0.75倍になる</t>
-  </si>
-  <si>
-    <t>火耐性</t>
-  </si>
-  <si>
-    <t>火耐性【大】/火耐性【小】/火耐性弱化</t>
-  </si>
-  <si>
-    <t>火耐性+20。合計耐性が25以上で火属性やられ小と大を無効化/火耐性+15。合計耐性が15以上で火属性やられ小を無効化/火耐性-20</t>
-  </si>
-  <si>
-    <t>風圧</t>
-  </si>
-  <si>
-    <t>風圧【大】無効/風圧【小】無効</t>
-  </si>
-  <si>
-    <t>風圧【大】と風圧【小】の影響を受けなくなる。龍風圧を風圧【大】の効果に軽減/風圧【小】の影響を受けなくなる</t>
-  </si>
-  <si>
-    <t>笛</t>
-  </si>
-  <si>
-    <t>笛吹き名人</t>
-  </si>
-  <si>
-    <t>狩猟笛の演奏の効果時間が延び、回復効果のある旋律は回復量が多い方の効果が出やすくなる。さらに笛アイテムが1/2の確率で壊れずに済む</t>
-  </si>
-  <si>
-    <t>紅兜</t>
-  </si>
-  <si>
-    <t>紅兜の魂</t>
-  </si>
-  <si>
-    <t>逆恨み + 集中</t>
-  </si>
-  <si>
-    <t>ベルナ</t>
-  </si>
-  <si>
-    <t>ベルナの心</t>
-  </si>
-  <si>
-    <t>火耐性【小】 + 腹減り半減</t>
-  </si>
-  <si>
-    <t>変則射撃</t>
-  </si>
-  <si>
-    <t>特定射撃強化</t>
-  </si>
-  <si>
-    <t>ボウガンの武器内蔵弾と弓の曲射、剛射の威力が1.2倍にアップ</t>
-  </si>
-  <si>
-    <t>防御</t>
-  </si>
-  <si>
-    <t>防御力UP【大】/防御力UP【中】/防御力UP【小】/防御力DOWN【小】/防御力DOWN【中】/防御力DOWN【大】</t>
-  </si>
-  <si>
-    <t>防御力1.06倍+25/防御力1.03倍+20/防御力+15/防御力-10。ただし1未満にはならない/防御力0.95倍-10。ただし1未満にはならない/防御力0.9倍-10。ただし1未満にはならない</t>
-  </si>
-  <si>
-    <t>砲術</t>
-  </si>
-  <si>
-    <t>砲術王/砲術師</t>
-  </si>
-  <si>
-    <t>バリスタ、ガンランスの砲撃、竜撃砲の威力が1.2倍になる。チャージアックスの榴弾ビン装着の属性開放斬りの威力が1.35倍、徹甲榴弾、竜撃弾、連爆榴弾、大砲弾の威力が1.3倍になる。竜撃砲の冷却時間が120秒から90秒に短縮される。またガンランスのヒートゲージ赤の変動が1/2になる/バリスタ、ガンランスの砲撃、竜撃砲の威力が1.1倍になる。チャージアックスの榴弾ビン装着の属性開放斬りの威力が1.3倍、徹甲榴弾、竜撃弾、連爆榴弾、大砲弾の威力が1.15倍になる。またガンランスのヒートゲージ赤の変動が2/3になる</t>
-  </si>
-  <si>
-    <t>捕獲</t>
-  </si>
-  <si>
-    <t>捕獲名人/捕獲達人</t>
-  </si>
-  <si>
-    <t>モンスター捕獲時の捕獲報酬枠が2～3枠から3～4枠に増える/モンスター捕獲時の捕獲報酬枠が2～3枠から3枠に増える</t>
-  </si>
-  <si>
-    <t>北辰納豆流</t>
-  </si>
-  <si>
-    <t>ネバネバ剣法</t>
-  </si>
-  <si>
-    <t>不屈 + ランナー + スタミナ奪取</t>
-  </si>
-  <si>
-    <t>矛砕</t>
-  </si>
-  <si>
-    <t>矛砕の魂</t>
-  </si>
-  <si>
-    <t>業物 + 反動軽減+2 + 精霊の加護</t>
-  </si>
-  <si>
-    <t>ポッケ</t>
-  </si>
-  <si>
-    <t>ポッケの心</t>
-  </si>
-  <si>
-    <t>氷耐性【小】 + まんぷく</t>
-  </si>
-  <si>
-    <t>本気</t>
-  </si>
-  <si>
-    <t>力の解放+2/力の解放+1</t>
-  </si>
-  <si>
-    <t>受けた合計ダメージが180ごとに、または大型モンスターに発見された状態が合計5分間になるたびに発動。1分30秒の間、会心率が50%上がり、スタミナ消費が1/4になる。スキルの挑戦者、フルチャージとは重複しない/受けた合計ダメージが180ごとに、または大型モンスターに発見された状態が合計5分間になるたびに発動。1分30秒の間、会心率が30%上がり、スタミナ消費が1/2になる。スキルの挑戦者、フルチャージとは重複しない</t>
-  </si>
-  <si>
-    <t>麻痺</t>
-  </si>
-  <si>
-    <t>麻痺無効/麻痺倍加</t>
-  </si>
-  <si>
-    <t>麻痺状態にならなくなる/麻痺状態の時間が2倍になる</t>
-  </si>
-  <si>
-    <t>麻痺瓶追加</t>
-  </si>
-  <si>
-    <t>麻痺ビン追加</t>
-  </si>
-  <si>
-    <t>麻痺ビンの装着が可能になる</t>
-  </si>
-  <si>
-    <t>水属性攻撃</t>
-  </si>
-  <si>
-    <t>水属性攻撃強化+2/水属性攻撃強化+1/水属性攻撃弱化</t>
-  </si>
-  <si>
-    <t>水属性の攻撃が1.1倍+6になる/水属性の攻撃が1.05倍+4になる/水属性の攻撃が0.75倍になる</t>
-  </si>
-  <si>
-    <t>水耐性</t>
-  </si>
-  <si>
-    <t>水耐性【大】/水耐性【小】/水耐性弱化</t>
-  </si>
-  <si>
-    <t>水耐性+20。合計耐性が25以上で水属性やられ小と大を無効化/水耐性+15。合計耐性が15以上で水属性やられ小を無効化/水耐性-20</t>
-  </si>
-  <si>
-    <t>無傷</t>
-  </si>
-  <si>
-    <t>フルチャージ</t>
-  </si>
-  <si>
-    <t>体力が最大の時に攻撃力+20。スキルの力の解放、挑戦者とは重複しない</t>
-  </si>
-  <si>
-    <t>無心</t>
-  </si>
-  <si>
-    <t>明鏡止水</t>
-  </si>
-  <si>
-    <t>狩技ゲージの溜まりやすさが1.15倍にアップ</t>
-  </si>
-  <si>
-    <t>野草知識</t>
-  </si>
-  <si>
-    <t>薬草超強化/薬草強化</t>
-  </si>
-  <si>
-    <t>薬草の回復力が50になる。広域化に関してはスキル所持者から仲間に対しては変化がないが、仲間からスキル所持者に対しては回復量が増える/薬草の回復力が30になる。広域化に関してはスキル所持者から仲間に対しては変化がないが、仲間からスキル所持者に対しては回復量が増える</t>
-  </si>
-  <si>
-    <t>ユクモ</t>
-  </si>
-  <si>
-    <t>ユクモの心</t>
-  </si>
-  <si>
-    <t>水耐性【小】 + ハニーハンター</t>
-  </si>
-  <si>
-    <t>鎧裂</t>
-  </si>
-  <si>
-    <t>鎧裂の魂</t>
-  </si>
-  <si>
-    <t>ガード性能+2 + 納刀術</t>
-  </si>
-  <si>
-    <t>龍気</t>
-  </si>
-  <si>
-    <t>龍気活性</t>
-  </si>
-  <si>
-    <t>体力が２/３以下になると、龍属性やられになるが、全ての属性耐性値が50になり攻撃力が1.1倍になる。龍属性やられは体力が戻ると回復する</t>
-  </si>
-  <si>
-    <t>龍識船</t>
-  </si>
-  <si>
-    <t>龍識船の心</t>
-  </si>
-  <si>
-    <t>龍耐性【小】 + 細菌研究家</t>
-  </si>
-  <si>
-    <t>龍属性攻撃</t>
-  </si>
-  <si>
-    <t>龍属性攻撃強化+2/龍属性攻撃強化+1/龍属性攻撃弱化</t>
-  </si>
-  <si>
-    <t>龍属性の攻撃が1.1倍+6になる/龍属性の攻撃が1.05倍+4になる/龍属性の攻撃が0.75倍になる</t>
-  </si>
-  <si>
-    <t>龍耐性</t>
-  </si>
-  <si>
-    <t>龍耐性【大】/龍耐性【小】/龍耐性弱化</t>
-  </si>
-  <si>
-    <t>龍耐性+20。合計耐性が25以上で龍属性やられ小と大を無効化/龍耐性+15。合計耐性が15以上で龍属性やられ小を無効化/龍耐性-20</t>
-  </si>
-  <si>
-    <t>榴弾追加</t>
-  </si>
-  <si>
-    <t>徹甲榴弾全LV追加/徹甲榴弾LV1追加</t>
-  </si>
-  <si>
-    <t>全LVの徹甲榴弾が使えるようになる/LV1徹甲榴弾が使えるようになる</t>
-  </si>
-  <si>
-    <t>裂傷</t>
-  </si>
-  <si>
-    <t>裂傷無効/裂傷倍加</t>
-  </si>
-  <si>
-    <t>裂傷状態にならなくなる/裂傷状態が2倍になる</t>
-  </si>
-  <si>
-    <t>連撃</t>
-  </si>
-  <si>
-    <t>連撃の心得</t>
-  </si>
-  <si>
-    <t>攻撃ヒットで5秒間会心率が25%上昇。その間に連続で攻撃が5回ヒットすると会心率上昇が30%になる</t>
+    <t>발도회심(抜刀会心)</t>
+  </si>
+  <si>
+    <t>발도술【기】(抜刀術【技】)</t>
+  </si>
+  <si>
+    <t>발도 공격 시에 회심률이 +100% 늘어난다.</t>
+  </si>
+  <si>
+    <t>발도멸기(抜刀減気)</t>
+  </si>
+  <si>
+    <t>발도술【력】(抜刀術【力】)</t>
+  </si>
+  <si>
+    <t>절단속성의 발도 공격 시에 공격력5와 멸기치15(쌍검은5)가 추가된다. 머리 공격 시에는 기절치 30도 추가</t>
+  </si>
+  <si>
+    <t>공복(腹減り)</t>
+  </si>
+  <si>
+    <t>공복 무효(腹減り無効)/공복 반감(腹減り半減)/공복 배가【소】(腹減り倍加【小】)/공복 배가【대】(腹減り倍加【大】)</t>
+  </si>
+  <si>
+    <t>공복에 의한 스태미너 감소가 없어진다./공복에 의한 스태미너 감소가 1/2이 된다./공복에 의한 스태미너 감소속도가 1.5배로 올라간다./공복에 의한 스태미너 감소속도가 2배로 올라간다.</t>
+  </si>
+  <si>
+    <t>반동(反動)</t>
+  </si>
+  <si>
+    <t>반동경감+3(反動軽減+3)/반동경감+2(反動軽減+2)/반동경감+1(反動軽減+1)/반동경감-1(反動軽減-1)/반동경감-2(反動軽減-2)/반동경감-3(反動軽減-3)</t>
+  </si>
+  <si>
+    <t>보우건의 반동이 3단계 작아진다. 속사의 반동에는 효과가 없다./보우건의 반동이 2단계 작아진다. 속사의 반동에는 효과가 없다./보우건의 반동이 1단계 작아진다. 속사의 반동에는 효과가 없다./보우건의 반동이 1단계 커진다. 속사의 반동에는 효과가 없다./보우건의 반동이 2단계 커진다. 속사의 반동에는 효과가 없다./보우건의 반동이 3단계 커진다. 속사의 반동에는 효과가 없다.</t>
+  </si>
+  <si>
+    <t>비행술집(飛行酒場)</t>
+  </si>
+  <si>
+    <t>비행술집의 마음(飛行酒場の心)</t>
+  </si>
+  <si>
+    <t>KO술(KO術) + 피리불기 명인(笛吹き名人)</t>
+  </si>
+  <si>
+    <t>비술(秘術)</t>
+  </si>
+  <si>
+    <t>스킬 가점+2(スキル加点+2)</t>
+  </si>
+  <si>
+    <t>장비하고 있는 스킬 포인트의 합계치에 +2가 된다.</t>
+  </si>
+  <si>
+    <t>화속성 공격(火属性攻撃)</t>
+  </si>
+  <si>
+    <t>화속성 공격강화+2(火属性攻撃強化+2)/화속성 공격강화+1(火属性攻撃強化+1)/화속성 공격약화(火属性攻撃弱化)</t>
+  </si>
+  <si>
+    <t>화속성의 공격이 1.1배+6이 된다./화속성의 공격이 1.05배+4이 된다./화속성의 공격이 0.75배가 된다.</t>
+  </si>
+  <si>
+    <t>화내성(火耐性)</t>
+  </si>
+  <si>
+    <t>화내성【대】(火耐性【大】)/화내성【소】(火耐性【小】)/화내성 약화(火耐性弱化)</t>
+  </si>
+  <si>
+    <t>화내성+20. 합계내성이 25이상이면 화속성 피해 소와 대를 무효화/화내성+15. 합계내성이 15이상이면 화속성 피해 소를 무효화/화내성-20</t>
+  </si>
+  <si>
+    <t>풍압(風圧)</t>
+  </si>
+  <si>
+    <t>풍압【대】 무효(風圧【大】無効)/풍압【소】 무효(風圧【小】無効)</t>
+  </si>
+  <si>
+    <t>풍압【대】와 풍압【소】의 영향을 받지 않게 된다. 용풍압을 풍압【대】의 효과로 경감/풍압【소】의 영향을 받지 않게 된다.</t>
+  </si>
+  <si>
+    <t>피리(笛)</t>
+  </si>
+  <si>
+    <t>피리불기 명인(笛吹き名人)</t>
+  </si>
+  <si>
+    <t>수렵적 연주의 효과시간이 늘어나고 회복효과가 있는 선율은 회복량이 많은 쪽의 효과가 나오기 쉬워진다. 또한 피리 아이템이 1/2의 확률로 부숴지지 않는다.</t>
+  </si>
+  <si>
+    <t>홍두(紅兜)</t>
+  </si>
+  <si>
+    <t>홍두의 혼(紅兜の魂)</t>
+  </si>
+  <si>
+    <t>앙심(逆恨み) + 집중(集中)</t>
+  </si>
+  <si>
+    <t>베르나(ベルナ)</t>
+  </si>
+  <si>
+    <t>베르나의 마음(ベルナの心)</t>
+  </si>
+  <si>
+    <t>화내성【소】(火耐性【小】) + 공복 반감(腹減り半減)</t>
+  </si>
+  <si>
+    <t>변칙사격(変則射撃)</t>
+  </si>
+  <si>
+    <t>특정사격강화(特定射撃強化)</t>
+  </si>
+  <si>
+    <t>보우건의 무기내장탄과 활의 곡사, 강사의 위력이 1.2배로 상승</t>
+  </si>
+  <si>
+    <t>방어(防御)</t>
+  </si>
+  <si>
+    <t>방어력UP【대】(防御力UP【大】)/방어력UP【중】(防御力UP【中】)/방어력UP【소】(防御力UP【小】)/방어력DOWN【소】(防御力DOWN【小】)/방어력DOWN【중】(防御力DOWN【中】)/방어력DOWN【대】(防御力DOWN【大】)</t>
+  </si>
+  <si>
+    <t>방어력 1.06배+25/방어력 1.03배+20/방어력+15/방어력-10. 단 1미만이 되지 않는다./방어력 0.95배-10. 단 1미만이 되지 않는다./방어력 0.9배-10. 단 1미만이 되지 않는다.</t>
+  </si>
+  <si>
+    <t>포술(砲術)</t>
+  </si>
+  <si>
+    <t>포술왕(砲術王)/포술사(砲術師)</t>
+  </si>
+  <si>
+    <t>발리스타, 건랜스의 포격, 용격포의 위력이 1.2배가 된다. 챠지 액스의 유탄병 장착 속성해방 베기의 위력이 1.35배, 철갑유탄, 용격탄, 연폭유탄, 대포탄의 위력이 1.3배가 된다. 용격포의 냉각시간이 120초에서 90초로 단축된다. 또 건랜스의 히트 게이지 빨강의 변동이 1/2가 된다./발리스타, 건랜스의 포격, 용격포의 위력이 1.1배가 된다. 챠지 액스의 유탄병 장착 속성해방 베기의 위력이 1.3배, 철갑유탄, 용격탄, 연폭유탄, 대포탄의 위력이 1.15배가 된다. 또 건랜스의 히트 게이지 빨강의 변동이 2/3가 된다.</t>
+  </si>
+  <si>
+    <t>포획(捕獲)</t>
+  </si>
+  <si>
+    <t>포획 명인(捕獲名人)/포획 달인(捕獲達人)</t>
+  </si>
+  <si>
+    <t>몬스터 포획 시의 포획보수칸이 2~3칸에서 3~4칸으로 늘어난다./몬스터 포획 시의 포획보수칸이 2~3칸에서 3칸으로 늘어난다.</t>
+  </si>
+  <si>
+    <t>북진낫토류(北辰納豆流)</t>
+  </si>
+  <si>
+    <t>끈적끈적 검법(ネバネバ剣法)</t>
+  </si>
+  <si>
+    <t>불굴(不屈) + 러너(ランナー) + 스태미너 탈취(スタミナ奪取)</t>
+  </si>
+  <si>
+    <t>모쇄(矛砕)</t>
+  </si>
+  <si>
+    <t>모쇄의 혼(矛砕の魂)</t>
+  </si>
+  <si>
+    <t>업물(業物) + 반동경감+2(反動軽減+2) + 정령의 가호(精霊の加護)</t>
+  </si>
+  <si>
+    <t>폿케(ポッケ)</t>
+  </si>
+  <si>
+    <t>폿케의 마음(ポッケの心)</t>
+  </si>
+  <si>
+    <t>빙내성【소】(氷耐性【小】) + 만복(まんぷく)</t>
+  </si>
+  <si>
+    <t>잠재력(本気)</t>
+  </si>
+  <si>
+    <t>힘의 해방+2(力の解放+2)/힘의 해방+1(力の解放+1)</t>
+  </si>
+  <si>
+    <t>받은 합계 데미지가 180간격으로, 혹은 대형 몬스터에게 발견된 상태가 합계 5분간이 될 때 마다 발동. 1분30초간, 회심률이 50% 오르고, 스태미너 소비가 1/4이 된다. 스킬 도전자(挑戦者), 풀차지(フルチャージ)와는 중복되지 않는다./받은 합계 데미지가 180간격으로, 혹은 대형 몬스터에게 발견된 상태가 합계 5분간이 될 때 마다 발동. 1분30초간, 회심률이 30% 오르고, 스태미너 소비가 1/2이 된다. 스킬 도전자(挑戦者), 풀차지(フルチャージ)와는 중복되지 않는다.</t>
+  </si>
+  <si>
+    <t>마비(麻痺)</t>
+  </si>
+  <si>
+    <t>마비 무효(麻痺無効)/마비 배가(麻痺倍加)</t>
+  </si>
+  <si>
+    <t>마비 상태가 되지 않는다./마비상태의 시간이 2배가 된다.</t>
+  </si>
+  <si>
+    <t>마비병추가(麻痺瓶追加)</t>
+  </si>
+  <si>
+    <t>마비병 추가(麻痺ビン追加)</t>
+  </si>
+  <si>
+    <t>마비병의 장착이 가능하게 된다.</t>
+  </si>
+  <si>
+    <t>수속성 공격(水属性攻撃)</t>
+  </si>
+  <si>
+    <t>수속성 공격강화+2(水属性攻撃強化+2)/수속성 공격강화+1(水属性攻撃強化+1)/수속성 공격약화(水属性攻撃弱化)</t>
+  </si>
+  <si>
+    <t>수속성의 공격이 1.1배+6이 된다./수속성의 공격이 1.05배+4가 된다./수속성의 공격이 0.75배가 된다.</t>
+  </si>
+  <si>
+    <t>수내성(水耐性)</t>
+  </si>
+  <si>
+    <t>수내성【대】(水耐性【大】)/수내성【소】(水耐性【小】)/수내성 약화(水耐性弱化)</t>
+  </si>
+  <si>
+    <t>수내성+20. 합계내성이 25이상이면 수속성 피해 소와 대를 무효화/수내성+15. 합계내성이 15이상이면 수속성 피해 소를 무효화/수내성-20</t>
+  </si>
+  <si>
+    <t>무상(無傷)</t>
+  </si>
+  <si>
+    <t>풀 챠지(フルチャージ)</t>
+  </si>
+  <si>
+    <t>체력이 최대일 때 공격력+20. 스킬 힘의해방(力の解放), 도전자(挑戦者)와 중복되지 않는다.</t>
+  </si>
+  <si>
+    <t>무심(無心)</t>
+  </si>
+  <si>
+    <t>명경지수(明鏡止水)</t>
+  </si>
+  <si>
+    <t>수기 게이지의 축적량이 1.15배로 상승</t>
+  </si>
+  <si>
+    <t>야초지식(野草知識)</t>
+  </si>
+  <si>
+    <t>약초 초강화(薬草超強化)/약초 강화(薬草強化)</t>
+  </si>
+  <si>
+    <t>약초의 회복력이 50이 된다. 광역화에 관해서는 스킬 소지자로부터 동료에 대한 변화는 없지만 동료로부터 스킬 소지자에 대한 회복량이 늘어난다./약초의 회복력이 30이 된다. 광역화에 관해서는 스킬 소지자로부터 동료에 대한 변화는 없지만 동료로부터 스킬 소지자에 대한 회복량이 늘어난다.</t>
+  </si>
+  <si>
+    <t>유쿠모(ユクモ)</t>
+  </si>
+  <si>
+    <t>유쿠모의 마음(ユクモの心)</t>
+  </si>
+  <si>
+    <t>수내성【소】(水耐性【小】) + 허니 헌터(ハニーハンター)</t>
+  </si>
+  <si>
+    <t>개열(鎧裂)</t>
+  </si>
+  <si>
+    <t>개열의 혼(鎧裂の魂)</t>
+  </si>
+  <si>
+    <t>가드 성능+2(ガード性能+2) + 납도술(納刀術)</t>
+  </si>
+  <si>
+    <t>용기(龍気)</t>
+  </si>
+  <si>
+    <t>용기활성(龍気活性)</t>
+  </si>
+  <si>
+    <t>체력이 2/3이하가 되면 용속성 피해상태가 되지만 모든 속성내성치가 50이 되고 공격력이 1.1배가 된다. 용속성 피해는 공격력이 돌아오면 회복된다.</t>
+  </si>
+  <si>
+    <t>용식선(龍識船)</t>
+  </si>
+  <si>
+    <t>용식선의 마음(龍識船の心)</t>
+  </si>
+  <si>
+    <t>용내성【소】(龍耐性【小】) + 세균연구가(細菌研究家)</t>
+  </si>
+  <si>
+    <t>용속성 공격(龍属性攻撃)</t>
+  </si>
+  <si>
+    <t>용속성 공격강화+2(龍属性攻撃強化+2)/용속성 공격강화+1(龍属性攻撃強化+1)/용속성 공격약화(龍属性攻撃弱化)</t>
+  </si>
+  <si>
+    <t>용속성의 공격이 1.1배+6이 된다./용속성의 공격이 1.05배+4가 된다./용속성의 공격이 0.75배가 된다.</t>
+  </si>
+  <si>
+    <t>용내성(龍耐性)</t>
+  </si>
+  <si>
+    <t>용내성【대】(龍耐性【大】)/용내성【소】(龍耐性【小】)/용내성 약화(龍耐性弱化)</t>
+  </si>
+  <si>
+    <t>용내성+20. 합계내성이 25이상이면 용속성 피해 소와 대를 무효화/용내성+15. 합계내성이 15이상이면 용속성 피해 소를 무효화/용내성-20</t>
+  </si>
+  <si>
+    <t>유탄추가(榴弾追加)</t>
+  </si>
+  <si>
+    <t>철갑유탄 전LV 추가(徹甲榴弾全LV追加)/철갑유탄 LV1 추가(徹甲榴弾LV1追加)</t>
+  </si>
+  <si>
+    <t>전LV의 철갑유탄을 사용할 수 있게 된다./LV1철갑유탄을 사용할 수 있게 된다.</t>
+  </si>
+  <si>
+    <t>열상(裂傷)</t>
+  </si>
+  <si>
+    <t>열상 무효(裂傷無効)/열상 배가(裂傷倍加)</t>
+  </si>
+  <si>
+    <t>열상 상태가 되지 않는다./열상상태가 2배가 된다.</t>
+  </si>
+  <si>
+    <t>연격(連撃)</t>
+  </si>
+  <si>
+    <t>연격의 심득(連撃の心得)</t>
+  </si>
+  <si>
+    <t>공격 명중 시 5초간 회심률이 25% 상승. 도중 연속으로 공격이 5회 명중하면 회심률 상승이 30%가 된다.</t>
   </si>
 </sst>
 </file>
@@ -2260,8 +2260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D159" workbookViewId="0">
-      <selection activeCell="D170" sqref="D170"/>
+    <sheetView tabSelected="1" topLeftCell="D196" workbookViewId="0">
+      <selection activeCell="D207" sqref="D207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>